<commit_message>
[MS-OXCNOTIF] fix case fail
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="180" windowWidth="15405" windowHeight="6780" tabRatio="570"/>
@@ -10,7 +10,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$1012</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$1010</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7200" uniqueCount="2298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7181" uniqueCount="2292">
   <si>
     <t>Req ID</t>
   </si>
@@ -7137,29 +7137,11 @@
   <si>
     <t>MS-OXCPRPT_R467</t>
   </si>
-  <si>
-    <t>MS-OXCPRPT_R466001</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OXCPRPT_R466001</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] When this is the first ROP RopGetPropertiesAll in the request buffer, and the maximum size of a ROP response buffer is used, and the serialized response would not fit, the implementation does fail the EcDoRpcExt2 method with a return value of 0x0000047D. &lt;5&gt; Section 3.2.5.2:  Exchange 2010 fails the EcDoRpcExt2 method with a return value of 0x0000047D.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] When this is the first ROP RopGetPropertiesAll in the request buffer, and the maximum size of a ROP response buffer is used, and the serialized response would not fit, the implementation does fail the EcDoRpcExt2 method with a return value of 0x000003F0. (Exchange 2007, Exchange 2013, Exchange 2016 follow this behavior).</t>
-  </si>
-  <si>
-    <t>MS-OXCPRPT_R466002</t>
-  </si>
-  <si>
-    <t>MS-OXCPRPT_R466:I, MS-OXCPRPT_R1:i</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7441,21 +7423,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7480,621 +7447,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="137">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
+  <dxfs count="61">
     <dxf>
       <font>
         <b val="0"/>
@@ -8433,6 +7805,228 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8562,34 +8156,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1012" tableType="xml" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135" connectionId="1">
-  <autoFilter ref="A19:I1012"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1010" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I1010"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="134">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="133">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="132">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="131">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="130">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="129">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="128">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="127">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="126">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8598,12 +8192,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="125" dataDxfId="123" headerRowBorderDxfId="124" tableBorderDxfId="122" totalsRowBorderDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="120"/>
-    <tableColumn id="2" name="Test" dataDxfId="119"/>
-    <tableColumn id="3" name="Description" dataDxfId="118"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8652,7 +8246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8685,9 +8279,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8720,6 +8331,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8897,15 +8525,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L1014"/>
+  <dimension ref="A1:L1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A923" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I928" sqref="I928"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
@@ -8954,127 +8580,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9087,12 +8713,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9105,12 +8731,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9123,12 +8749,12 @@
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9141,60 +8767,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -25872,11 +25498,9 @@
         <v>15</v>
       </c>
       <c r="H679" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I679" s="31" t="s">
-        <v>2293</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I679" s="20"/>
     </row>
     <row r="680" spans="1:9" ht="45">
       <c r="A680" s="29" t="s">
@@ -25899,7 +25523,7 @@
         <v>15</v>
       </c>
       <c r="H680" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I680" s="31"/>
     </row>
@@ -32161,18 +31785,18 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="927" spans="1:9" ht="75">
+    <row r="927" spans="1:9" ht="45">
       <c r="A927" s="29" t="s">
-        <v>2292</v>
+        <v>949</v>
       </c>
       <c r="B927" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C927" s="31" t="s">
-        <v>2294</v>
+        <v>2045</v>
       </c>
       <c r="D927" s="29" t="s">
-        <v>2297</v>
+        <v>2162</v>
       </c>
       <c r="E927" s="29" t="s">
         <v>22</v>
@@ -32190,18 +31814,18 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="928" spans="1:9" ht="60">
+    <row r="928" spans="1:9" ht="45">
       <c r="A928" s="29" t="s">
-        <v>2296</v>
+        <v>950</v>
       </c>
       <c r="B928" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C928" s="31" t="s">
-        <v>2295</v>
+        <v>2269</v>
       </c>
       <c r="D928" s="29" t="s">
-        <v>2297</v>
+        <v>2162</v>
       </c>
       <c r="E928" s="29" t="s">
         <v>22</v>
@@ -32221,16 +31845,16 @@
     </row>
     <row r="929" spans="1:9" ht="45">
       <c r="A929" s="29" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B929" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C929" s="31" t="s">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="D929" s="29" t="s">
-        <v>2162</v>
+        <v>2163</v>
       </c>
       <c r="E929" s="29" t="s">
         <v>22</v>
@@ -32250,16 +31874,16 @@
     </row>
     <row r="930" spans="1:9" ht="45">
       <c r="A930" s="29" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B930" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C930" s="31" t="s">
-        <v>2269</v>
+        <v>2270</v>
       </c>
       <c r="D930" s="29" t="s">
-        <v>2162</v>
+        <v>2163</v>
       </c>
       <c r="E930" s="29" t="s">
         <v>22</v>
@@ -32279,16 +31903,16 @@
     </row>
     <row r="931" spans="1:9" ht="45">
       <c r="A931" s="29" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B931" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C931" s="31" t="s">
-        <v>2046</v>
+        <v>2271</v>
       </c>
       <c r="D931" s="29" t="s">
-        <v>2163</v>
+        <v>2164</v>
       </c>
       <c r="E931" s="29" t="s">
         <v>22</v>
@@ -32308,16 +31932,16 @@
     </row>
     <row r="932" spans="1:9" ht="45">
       <c r="A932" s="29" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="B932" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C932" s="31" t="s">
-        <v>2270</v>
+        <v>2047</v>
       </c>
       <c r="D932" s="29" t="s">
-        <v>2163</v>
+        <v>2165</v>
       </c>
       <c r="E932" s="29" t="s">
         <v>22</v>
@@ -32329,24 +31953,24 @@
         <v>15</v>
       </c>
       <c r="H932" s="29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I932" s="31" t="s">
         <v>2236</v>
       </c>
     </row>
-    <row r="933" spans="1:9" ht="45">
+    <row r="933" spans="1:9" ht="60">
       <c r="A933" s="29" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B933" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C933" s="31" t="s">
-        <v>2271</v>
+        <v>2048</v>
       </c>
       <c r="D933" s="29" t="s">
-        <v>2164</v>
+        <v>2166</v>
       </c>
       <c r="E933" s="29" t="s">
         <v>22</v>
@@ -32358,7 +31982,7 @@
         <v>15</v>
       </c>
       <c r="H933" s="29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I933" s="31" t="s">
         <v>2236</v>
@@ -32366,16 +31990,16 @@
     </row>
     <row r="934" spans="1:9" ht="45">
       <c r="A934" s="29" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="B934" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C934" s="31" t="s">
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="D934" s="29" t="s">
-        <v>2165</v>
+        <v>2167</v>
       </c>
       <c r="E934" s="29" t="s">
         <v>22</v>
@@ -32393,18 +32017,18 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="935" spans="1:9" ht="60">
+    <row r="935" spans="1:9" ht="45">
       <c r="A935" s="29" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B935" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C935" s="31" t="s">
-        <v>2048</v>
+        <v>2050</v>
       </c>
       <c r="D935" s="29" t="s">
-        <v>2166</v>
+        <v>2167</v>
       </c>
       <c r="E935" s="29" t="s">
         <v>22</v>
@@ -32424,16 +32048,16 @@
     </row>
     <row r="936" spans="1:9" ht="45">
       <c r="A936" s="29" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="B936" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C936" s="31" t="s">
-        <v>2049</v>
+        <v>2051</v>
       </c>
       <c r="D936" s="29" t="s">
-        <v>2167</v>
+        <v>2168</v>
       </c>
       <c r="E936" s="29" t="s">
         <v>22</v>
@@ -32451,18 +32075,18 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="937" spans="1:9" ht="45">
+    <row r="937" spans="1:9" ht="75">
       <c r="A937" s="29" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B937" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C937" s="31" t="s">
-        <v>2050</v>
+        <v>2052</v>
       </c>
       <c r="D937" s="29" t="s">
-        <v>2167</v>
+        <v>2169</v>
       </c>
       <c r="E937" s="29" t="s">
         <v>22</v>
@@ -32482,16 +32106,16 @@
     </row>
     <row r="938" spans="1:9" ht="45">
       <c r="A938" s="29" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B938" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C938" s="31" t="s">
-        <v>2051</v>
+        <v>2053</v>
       </c>
       <c r="D938" s="29" t="s">
-        <v>2168</v>
+        <v>2170</v>
       </c>
       <c r="E938" s="29" t="s">
         <v>22</v>
@@ -32503,24 +32127,24 @@
         <v>15</v>
       </c>
       <c r="H938" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I938" s="31" t="s">
         <v>2236</v>
       </c>
     </row>
-    <row r="939" spans="1:9" ht="75">
+    <row r="939" spans="1:9" ht="45">
       <c r="A939" s="29" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B939" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C939" s="31" t="s">
-        <v>2052</v>
+        <v>2272</v>
       </c>
       <c r="D939" s="29" t="s">
-        <v>2169</v>
+        <v>2170</v>
       </c>
       <c r="E939" s="29" t="s">
         <v>22</v>
@@ -32532,24 +32156,24 @@
         <v>15</v>
       </c>
       <c r="H939" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I939" s="31" t="s">
         <v>2236</v>
       </c>
     </row>
-    <row r="940" spans="1:9" ht="45">
+    <row r="940" spans="1:9" ht="60">
       <c r="A940" s="29" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="B940" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C940" s="31" t="s">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="D940" s="29" t="s">
-        <v>2170</v>
+        <v>2171</v>
       </c>
       <c r="E940" s="29" t="s">
         <v>22</v>
@@ -32561,7 +32185,7 @@
         <v>15</v>
       </c>
       <c r="H940" s="29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I940" s="31" t="s">
         <v>2236</v>
@@ -32569,16 +32193,16 @@
     </row>
     <row r="941" spans="1:9" ht="45">
       <c r="A941" s="29" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="B941" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C941" s="31" t="s">
-        <v>2272</v>
+        <v>2055</v>
       </c>
       <c r="D941" s="29" t="s">
-        <v>2170</v>
+        <v>2172</v>
       </c>
       <c r="E941" s="29" t="s">
         <v>22</v>
@@ -32596,18 +32220,18 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="942" spans="1:9" ht="60">
+    <row r="942" spans="1:9" ht="45">
       <c r="A942" s="29" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="B942" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C942" s="31" t="s">
-        <v>2054</v>
+        <v>2056</v>
       </c>
       <c r="D942" s="29" t="s">
-        <v>2171</v>
+        <v>2173</v>
       </c>
       <c r="E942" s="29" t="s">
         <v>22</v>
@@ -32627,28 +32251,28 @@
     </row>
     <row r="943" spans="1:9" ht="45">
       <c r="A943" s="29" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="B943" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C943" s="31" t="s">
-        <v>2055</v>
+        <v>2057</v>
       </c>
       <c r="D943" s="29" t="s">
-        <v>2172</v>
+        <v>2174</v>
       </c>
       <c r="E943" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F943" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G943" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H943" s="29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I943" s="31" t="s">
         <v>2236</v>
@@ -32656,16 +32280,16 @@
     </row>
     <row r="944" spans="1:9" ht="45">
       <c r="A944" s="29" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B944" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C944" s="31" t="s">
-        <v>2056</v>
+        <v>2058</v>
       </c>
       <c r="D944" s="29" t="s">
-        <v>2173</v>
+        <v>2175</v>
       </c>
       <c r="E944" s="29" t="s">
         <v>22</v>
@@ -32677,7 +32301,7 @@
         <v>15</v>
       </c>
       <c r="H944" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I944" s="31" t="s">
         <v>2236</v>
@@ -32685,45 +32309,43 @@
     </row>
     <row r="945" spans="1:9" ht="45">
       <c r="A945" s="29" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="B945" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C945" s="31" t="s">
-        <v>2057</v>
+        <v>2273</v>
       </c>
       <c r="D945" s="29" t="s">
-        <v>2174</v>
+        <v>2176</v>
       </c>
       <c r="E945" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F945" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G945" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H945" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I945" s="31" t="s">
-        <v>2236</v>
-      </c>
-    </row>
-    <row r="946" spans="1:9" ht="45">
+        <v>18</v>
+      </c>
+      <c r="I945" s="31"/>
+    </row>
+    <row r="946" spans="1:9" ht="60">
       <c r="A946" s="29" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B946" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C946" s="31" t="s">
-        <v>2058</v>
+        <v>2274</v>
       </c>
       <c r="D946" s="29" t="s">
-        <v>2175</v>
+        <v>2176</v>
       </c>
       <c r="E946" s="29" t="s">
         <v>22</v>
@@ -32735,7 +32357,7 @@
         <v>15</v>
       </c>
       <c r="H946" s="29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I946" s="31" t="s">
         <v>2236</v>
@@ -32743,13 +32365,13 @@
     </row>
     <row r="947" spans="1:9" ht="45">
       <c r="A947" s="29" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="B947" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C947" s="31" t="s">
-        <v>2273</v>
+        <v>2275</v>
       </c>
       <c r="D947" s="29" t="s">
         <v>2176</v>
@@ -32764,22 +32386,24 @@
         <v>15</v>
       </c>
       <c r="H947" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I947" s="31"/>
-    </row>
-    <row r="948" spans="1:9" ht="60">
+        <v>21</v>
+      </c>
+      <c r="I947" s="31" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="948" spans="1:9" ht="45">
       <c r="A948" s="29" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B948" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C948" s="31" t="s">
-        <v>2274</v>
+        <v>2276</v>
       </c>
       <c r="D948" s="29" t="s">
-        <v>2176</v>
+        <v>2177</v>
       </c>
       <c r="E948" s="29" t="s">
         <v>22</v>
@@ -32791,24 +32415,22 @@
         <v>15</v>
       </c>
       <c r="H948" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I948" s="31" t="s">
-        <v>2236</v>
-      </c>
-    </row>
-    <row r="949" spans="1:9" ht="45">
+        <v>18</v>
+      </c>
+      <c r="I948" s="31"/>
+    </row>
+    <row r="949" spans="1:9" ht="60">
       <c r="A949" s="29" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="B949" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C949" s="31" t="s">
-        <v>2275</v>
+        <v>2277</v>
       </c>
       <c r="D949" s="29" t="s">
-        <v>2176</v>
+        <v>2177</v>
       </c>
       <c r="E949" s="29" t="s">
         <v>22</v>
@@ -32820,21 +32442,19 @@
         <v>15</v>
       </c>
       <c r="H949" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I949" s="31" t="s">
-        <v>2236</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I949" s="31"/>
     </row>
     <row r="950" spans="1:9" ht="45">
       <c r="A950" s="29" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="B950" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C950" s="31" t="s">
-        <v>2276</v>
+        <v>2278</v>
       </c>
       <c r="D950" s="29" t="s">
         <v>2177</v>
@@ -32853,18 +32473,18 @@
       </c>
       <c r="I950" s="31"/>
     </row>
-    <row r="951" spans="1:9" ht="60">
+    <row r="951" spans="1:9" ht="45">
       <c r="A951" s="29" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="B951" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C951" s="31" t="s">
-        <v>2277</v>
+        <v>2279</v>
       </c>
       <c r="D951" s="29" t="s">
-        <v>2177</v>
+        <v>2175</v>
       </c>
       <c r="E951" s="29" t="s">
         <v>22</v>
@@ -32876,22 +32496,24 @@
         <v>15</v>
       </c>
       <c r="H951" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I951" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="I951" s="31" t="s">
+        <v>2236</v>
+      </c>
     </row>
     <row r="952" spans="1:9" ht="45">
       <c r="A952" s="29" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="B952" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C952" s="31" t="s">
-        <v>2278</v>
+        <v>2280</v>
       </c>
       <c r="D952" s="29" t="s">
-        <v>2177</v>
+        <v>2178</v>
       </c>
       <c r="E952" s="29" t="s">
         <v>22</v>
@@ -32909,16 +32531,16 @@
     </row>
     <row r="953" spans="1:9" ht="45">
       <c r="A953" s="29" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="B953" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C953" s="31" t="s">
-        <v>2279</v>
+        <v>2281</v>
       </c>
       <c r="D953" s="29" t="s">
-        <v>2175</v>
+        <v>2178</v>
       </c>
       <c r="E953" s="29" t="s">
         <v>22</v>
@@ -32938,17 +32560,15 @@
     </row>
     <row r="954" spans="1:9" ht="45">
       <c r="A954" s="29" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="B954" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C954" s="31" t="s">
-        <v>2280</v>
-      </c>
-      <c r="D954" s="29" t="s">
-        <v>2178</v>
-      </c>
+        <v>2282</v>
+      </c>
+      <c r="D954" s="29"/>
       <c r="E954" s="29" t="s">
         <v>22</v>
       </c>
@@ -32959,22 +32579,22 @@
         <v>15</v>
       </c>
       <c r="H954" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I954" s="31"/>
     </row>
     <row r="955" spans="1:9" ht="45">
       <c r="A955" s="29" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="B955" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C955" s="31" t="s">
-        <v>2281</v>
+        <v>2059</v>
       </c>
       <c r="D955" s="29" t="s">
-        <v>2178</v>
+        <v>2179</v>
       </c>
       <c r="E955" s="29" t="s">
         <v>22</v>
@@ -32986,7 +32606,7 @@
         <v>15</v>
       </c>
       <c r="H955" s="29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I955" s="31" t="s">
         <v>2236</v>
@@ -32994,15 +32614,17 @@
     </row>
     <row r="956" spans="1:9" ht="45">
       <c r="A956" s="29" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="B956" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C956" s="31" t="s">
-        <v>2282</v>
-      </c>
-      <c r="D956" s="29"/>
+        <v>2060</v>
+      </c>
+      <c r="D956" s="29" t="s">
+        <v>2180</v>
+      </c>
       <c r="E956" s="29" t="s">
         <v>22</v>
       </c>
@@ -33013,22 +32635,24 @@
         <v>15</v>
       </c>
       <c r="H956" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I956" s="31"/>
+        <v>21</v>
+      </c>
+      <c r="I956" s="31" t="s">
+        <v>2236</v>
+      </c>
     </row>
     <row r="957" spans="1:9" ht="45">
       <c r="A957" s="29" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B957" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C957" s="31" t="s">
-        <v>2059</v>
+        <v>2061</v>
       </c>
       <c r="D957" s="29" t="s">
-        <v>2179</v>
+        <v>2181</v>
       </c>
       <c r="E957" s="29" t="s">
         <v>22</v>
@@ -33048,16 +32672,16 @@
     </row>
     <row r="958" spans="1:9" ht="45">
       <c r="A958" s="29" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="B958" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C958" s="31" t="s">
-        <v>2060</v>
+        <v>2062</v>
       </c>
       <c r="D958" s="29" t="s">
-        <v>2180</v>
+        <v>2182</v>
       </c>
       <c r="E958" s="29" t="s">
         <v>22</v>
@@ -33069,24 +32693,22 @@
         <v>15</v>
       </c>
       <c r="H958" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I958" s="31" t="s">
-        <v>2236</v>
-      </c>
-    </row>
-    <row r="959" spans="1:9" ht="45">
+        <v>18</v>
+      </c>
+      <c r="I958" s="31"/>
+    </row>
+    <row r="959" spans="1:9" ht="30">
       <c r="A959" s="29" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="B959" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C959" s="31" t="s">
-        <v>2061</v>
+        <v>2063</v>
       </c>
       <c r="D959" s="29" t="s">
-        <v>2181</v>
+        <v>2183</v>
       </c>
       <c r="E959" s="29" t="s">
         <v>22</v>
@@ -33098,24 +32720,22 @@
         <v>15</v>
       </c>
       <c r="H959" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I959" s="31" t="s">
-        <v>2236</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I959" s="31"/>
     </row>
     <row r="960" spans="1:9" ht="45">
       <c r="A960" s="29" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="B960" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C960" s="31" t="s">
-        <v>2062</v>
+        <v>2283</v>
       </c>
       <c r="D960" s="29" t="s">
-        <v>2182</v>
+        <v>2183</v>
       </c>
       <c r="E960" s="29" t="s">
         <v>22</v>
@@ -33127,22 +32747,24 @@
         <v>15</v>
       </c>
       <c r="H960" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I960" s="31"/>
+        <v>21</v>
+      </c>
+      <c r="I960" s="31" t="s">
+        <v>2236</v>
+      </c>
     </row>
     <row r="961" spans="1:10" ht="30">
       <c r="A961" s="29" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="B961" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C961" s="31" t="s">
-        <v>2063</v>
+        <v>2064</v>
       </c>
       <c r="D961" s="29" t="s">
-        <v>2183</v>
+        <v>2184</v>
       </c>
       <c r="E961" s="29" t="s">
         <v>22</v>
@@ -33160,16 +32782,16 @@
     </row>
     <row r="962" spans="1:10" ht="45">
       <c r="A962" s="29" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="B962" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C962" s="31" t="s">
-        <v>2283</v>
+        <v>2284</v>
       </c>
       <c r="D962" s="29" t="s">
-        <v>2183</v>
+        <v>2184</v>
       </c>
       <c r="E962" s="29" t="s">
         <v>22</v>
@@ -33189,16 +32811,16 @@
     </row>
     <row r="963" spans="1:10" ht="30">
       <c r="A963" s="29" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B963" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C963" s="31" t="s">
-        <v>2064</v>
+        <v>2065</v>
       </c>
       <c r="D963" s="29" t="s">
-        <v>2184</v>
+        <v>2185</v>
       </c>
       <c r="E963" s="29" t="s">
         <v>22</v>
@@ -33216,16 +32838,16 @@
     </row>
     <row r="964" spans="1:10" ht="45">
       <c r="A964" s="29" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="B964" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C964" s="31" t="s">
-        <v>2284</v>
+        <v>2285</v>
       </c>
       <c r="D964" s="29" t="s">
-        <v>2184</v>
+        <v>2185</v>
       </c>
       <c r="E964" s="29" t="s">
         <v>22</v>
@@ -33245,16 +32867,16 @@
     </row>
     <row r="965" spans="1:10" ht="30">
       <c r="A965" s="29" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B965" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C965" s="31" t="s">
-        <v>2065</v>
+        <v>2066</v>
       </c>
       <c r="D965" s="29" t="s">
-        <v>2185</v>
+        <v>2186</v>
       </c>
       <c r="E965" s="29" t="s">
         <v>22</v>
@@ -33272,16 +32894,16 @@
     </row>
     <row r="966" spans="1:10" ht="45">
       <c r="A966" s="29" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="B966" s="30" t="s">
         <v>1150</v>
       </c>
       <c r="C966" s="31" t="s">
-        <v>2285</v>
+        <v>2286</v>
       </c>
       <c r="D966" s="29" t="s">
-        <v>2185</v>
+        <v>2186</v>
       </c>
       <c r="E966" s="29" t="s">
         <v>22</v>
@@ -33299,51 +32921,50 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="967" spans="1:10" ht="30">
-      <c r="A967" s="29" t="s">
-        <v>987</v>
-      </c>
-      <c r="B967" s="30" t="s">
-        <v>1150</v>
+    <row r="967" spans="1:10" ht="45">
+      <c r="A967" s="30" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B967" s="33">
+        <v>6</v>
       </c>
       <c r="C967" s="31" t="s">
-        <v>2066</v>
-      </c>
-      <c r="D967" s="29" t="s">
-        <v>2186</v>
-      </c>
+        <v>2287</v>
+      </c>
+      <c r="D967" s="29"/>
       <c r="E967" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F967" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G967" s="29" t="s">
+      <c r="G967" s="34" t="s">
         <v>15</v>
       </c>
       <c r="H967" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I967" s="31"/>
-    </row>
-    <row r="968" spans="1:10" ht="45">
+        <v>21</v>
+      </c>
+      <c r="I967" s="35" t="s">
+        <v>2236</v>
+      </c>
+      <c r="J967" s="31"/>
+    </row>
+    <row r="968" spans="1:10" ht="30">
       <c r="A968" s="29" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B968" s="30" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="C968" s="31" t="s">
-        <v>2286</v>
-      </c>
-      <c r="D968" s="29" t="s">
-        <v>2186</v>
-      </c>
+        <v>2067</v>
+      </c>
+      <c r="D968" s="29"/>
       <c r="E968" s="29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F968" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G968" s="29" t="s">
         <v>15</v>
@@ -33351,47 +32972,42 @@
       <c r="H968" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I968" s="31" t="s">
-        <v>2236</v>
-      </c>
-    </row>
-    <row r="969" spans="1:10" ht="45">
-      <c r="A969" s="30" t="s">
-        <v>2251</v>
-      </c>
-      <c r="B969" s="33">
-        <v>6</v>
+      <c r="I968" s="31"/>
+    </row>
+    <row r="969" spans="1:10" ht="30">
+      <c r="A969" s="29" t="s">
+        <v>990</v>
+      </c>
+      <c r="B969" s="30" t="s">
+        <v>1151</v>
       </c>
       <c r="C969" s="31" t="s">
-        <v>2287</v>
+        <v>2068</v>
       </c>
       <c r="D969" s="29"/>
       <c r="E969" s="29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F969" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G969" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G969" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H969" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I969" s="35" t="s">
-        <v>2236</v>
-      </c>
-      <c r="J969" s="31"/>
+      <c r="I969" s="31"/>
     </row>
     <row r="970" spans="1:10" ht="30">
       <c r="A970" s="29" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B970" s="30" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="C970" s="31" t="s">
-        <v>2067</v>
+        <v>2069</v>
       </c>
       <c r="D970" s="29"/>
       <c r="E970" s="29" t="s">
@@ -33408,15 +33024,15 @@
       </c>
       <c r="I970" s="31"/>
     </row>
-    <row r="971" spans="1:10" ht="30">
+    <row r="971" spans="1:10" ht="60">
       <c r="A971" s="29" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="B971" s="30" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="C971" s="31" t="s">
-        <v>2068</v>
+        <v>2070</v>
       </c>
       <c r="D971" s="29"/>
       <c r="E971" s="29" t="s">
@@ -33435,13 +33051,13 @@
     </row>
     <row r="972" spans="1:10" ht="30">
       <c r="A972" s="29" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="B972" s="30" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="C972" s="31" t="s">
-        <v>2069</v>
+        <v>2071</v>
       </c>
       <c r="D972" s="29"/>
       <c r="E972" s="29" t="s">
@@ -33458,15 +33074,15 @@
       </c>
       <c r="I972" s="31"/>
     </row>
-    <row r="973" spans="1:10" ht="60">
+    <row r="973" spans="1:10" ht="30">
       <c r="A973" s="29" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="B973" s="30" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="C973" s="31" t="s">
-        <v>2070</v>
+        <v>2072</v>
       </c>
       <c r="D973" s="29"/>
       <c r="E973" s="29" t="s">
@@ -33485,13 +33101,13 @@
     </row>
     <row r="974" spans="1:10" ht="30">
       <c r="A974" s="29" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="B974" s="30" t="s">
         <v>1153</v>
       </c>
       <c r="C974" s="31" t="s">
-        <v>2071</v>
+        <v>2073</v>
       </c>
       <c r="D974" s="29"/>
       <c r="E974" s="29" t="s">
@@ -33510,13 +33126,13 @@
     </row>
     <row r="975" spans="1:10" ht="30">
       <c r="A975" s="29" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="B975" s="30" t="s">
         <v>1153</v>
       </c>
       <c r="C975" s="31" t="s">
-        <v>2072</v>
+        <v>2074</v>
       </c>
       <c r="D975" s="29"/>
       <c r="E975" s="29" t="s">
@@ -33535,13 +33151,13 @@
     </row>
     <row r="976" spans="1:10" ht="30">
       <c r="A976" s="29" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B976" s="30" t="s">
         <v>1153</v>
       </c>
       <c r="C976" s="31" t="s">
-        <v>2073</v>
+        <v>2075</v>
       </c>
       <c r="D976" s="29"/>
       <c r="E976" s="29" t="s">
@@ -33558,15 +33174,15 @@
       </c>
       <c r="I976" s="31"/>
     </row>
-    <row r="977" spans="1:9" ht="30">
+    <row r="977" spans="1:9" ht="45">
       <c r="A977" s="29" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="B977" s="30" t="s">
         <v>1153</v>
       </c>
       <c r="C977" s="31" t="s">
-        <v>2074</v>
+        <v>2076</v>
       </c>
       <c r="D977" s="29"/>
       <c r="E977" s="29" t="s">
@@ -33583,15 +33199,15 @@
       </c>
       <c r="I977" s="31"/>
     </row>
-    <row r="978" spans="1:9" ht="30">
+    <row r="978" spans="1:9">
       <c r="A978" s="29" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B978" s="30" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="C978" s="31" t="s">
-        <v>2075</v>
+        <v>2077</v>
       </c>
       <c r="D978" s="29"/>
       <c r="E978" s="29" t="s">
@@ -33608,15 +33224,15 @@
       </c>
       <c r="I978" s="31"/>
     </row>
-    <row r="979" spans="1:9" ht="45">
+    <row r="979" spans="1:9" ht="30">
       <c r="A979" s="29" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="B979" s="30" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="C979" s="31" t="s">
-        <v>2076</v>
+        <v>2078</v>
       </c>
       <c r="D979" s="29"/>
       <c r="E979" s="29" t="s">
@@ -33635,13 +33251,13 @@
     </row>
     <row r="980" spans="1:9">
       <c r="A980" s="29" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B980" s="30" t="s">
         <v>1154</v>
       </c>
       <c r="C980" s="31" t="s">
-        <v>2077</v>
+        <v>2079</v>
       </c>
       <c r="D980" s="29"/>
       <c r="E980" s="29" t="s">
@@ -33658,15 +33274,15 @@
       </c>
       <c r="I980" s="31"/>
     </row>
-    <row r="981" spans="1:9" ht="30">
+    <row r="981" spans="1:9" ht="120">
       <c r="A981" s="29" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="B981" s="30" t="s">
         <v>1154</v>
       </c>
       <c r="C981" s="31" t="s">
-        <v>2078</v>
+        <v>2080</v>
       </c>
       <c r="D981" s="29"/>
       <c r="E981" s="29" t="s">
@@ -33683,22 +33299,22 @@
       </c>
       <c r="I981" s="31"/>
     </row>
-    <row r="982" spans="1:9">
+    <row r="982" spans="1:9" ht="30">
       <c r="A982" s="29" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B982" s="30" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="C982" s="31" t="s">
-        <v>2079</v>
+        <v>2081</v>
       </c>
       <c r="D982" s="29"/>
       <c r="E982" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F982" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G982" s="29" t="s">
         <v>15</v>
@@ -33708,15 +33324,15 @@
       </c>
       <c r="I982" s="31"/>
     </row>
-    <row r="983" spans="1:9" ht="120">
+    <row r="983" spans="1:9" ht="30">
       <c r="A983" s="29" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="B983" s="30" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="C983" s="31" t="s">
-        <v>2080</v>
+        <v>2082</v>
       </c>
       <c r="D983" s="29"/>
       <c r="E983" s="29" t="s">
@@ -33735,20 +33351,20 @@
     </row>
     <row r="984" spans="1:9" ht="30">
       <c r="A984" s="29" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="B984" s="30" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="C984" s="31" t="s">
-        <v>2081</v>
+        <v>2083</v>
       </c>
       <c r="D984" s="29"/>
       <c r="E984" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F984" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G984" s="29" t="s">
         <v>15</v>
@@ -33758,15 +33374,15 @@
       </c>
       <c r="I984" s="31"/>
     </row>
-    <row r="985" spans="1:9" ht="30">
+    <row r="985" spans="1:9" ht="45">
       <c r="A985" s="29" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="B985" s="30" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="C985" s="31" t="s">
-        <v>2082</v>
+        <v>2084</v>
       </c>
       <c r="D985" s="29"/>
       <c r="E985" s="29" t="s">
@@ -33785,13 +33401,13 @@
     </row>
     <row r="986" spans="1:9" ht="30">
       <c r="A986" s="29" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B986" s="30" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="C986" s="31" t="s">
-        <v>2083</v>
+        <v>2085</v>
       </c>
       <c r="D986" s="29"/>
       <c r="E986" s="29" t="s">
@@ -33808,15 +33424,15 @@
       </c>
       <c r="I986" s="31"/>
     </row>
-    <row r="987" spans="1:9" ht="45">
+    <row r="987" spans="1:9" ht="30">
       <c r="A987" s="29" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B987" s="30" t="s">
         <v>1157</v>
       </c>
       <c r="C987" s="31" t="s">
-        <v>2084</v>
+        <v>2086</v>
       </c>
       <c r="D987" s="29"/>
       <c r="E987" s="29" t="s">
@@ -33833,15 +33449,15 @@
       </c>
       <c r="I987" s="31"/>
     </row>
-    <row r="988" spans="1:9" ht="30">
+    <row r="988" spans="1:9" ht="60">
       <c r="A988" s="29" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B988" s="30" t="s">
         <v>1157</v>
       </c>
       <c r="C988" s="31" t="s">
-        <v>2085</v>
+        <v>2087</v>
       </c>
       <c r="D988" s="29"/>
       <c r="E988" s="29" t="s">
@@ -33858,15 +33474,15 @@
       </c>
       <c r="I988" s="31"/>
     </row>
-    <row r="989" spans="1:9" ht="30">
+    <row r="989" spans="1:9" ht="45">
       <c r="A989" s="29" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B989" s="30" t="s">
         <v>1157</v>
       </c>
       <c r="C989" s="31" t="s">
-        <v>2086</v>
+        <v>2088</v>
       </c>
       <c r="D989" s="29"/>
       <c r="E989" s="29" t="s">
@@ -33883,15 +33499,15 @@
       </c>
       <c r="I989" s="31"/>
     </row>
-    <row r="990" spans="1:9" ht="60">
+    <row r="990" spans="1:9" ht="75">
       <c r="A990" s="29" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B990" s="30" t="s">
         <v>1157</v>
       </c>
       <c r="C990" s="31" t="s">
-        <v>2087</v>
+        <v>2089</v>
       </c>
       <c r="D990" s="29"/>
       <c r="E990" s="29" t="s">
@@ -33910,13 +33526,13 @@
     </row>
     <row r="991" spans="1:9" ht="45">
       <c r="A991" s="29" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="B991" s="30" t="s">
         <v>1157</v>
       </c>
       <c r="C991" s="31" t="s">
-        <v>2088</v>
+        <v>2090</v>
       </c>
       <c r="D991" s="29"/>
       <c r="E991" s="29" t="s">
@@ -33933,15 +33549,15 @@
       </c>
       <c r="I991" s="31"/>
     </row>
-    <row r="992" spans="1:9" ht="75">
+    <row r="992" spans="1:9" ht="45">
       <c r="A992" s="29" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B992" s="30" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="C992" s="31" t="s">
-        <v>2089</v>
+        <v>2091</v>
       </c>
       <c r="D992" s="29"/>
       <c r="E992" s="29" t="s">
@@ -33958,15 +33574,15 @@
       </c>
       <c r="I992" s="31"/>
     </row>
-    <row r="993" spans="1:9" ht="45">
+    <row r="993" spans="1:9">
       <c r="A993" s="29" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="B993" s="30" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="C993" s="31" t="s">
-        <v>2090</v>
+        <v>2092</v>
       </c>
       <c r="D993" s="29"/>
       <c r="E993" s="29" t="s">
@@ -33983,15 +33599,15 @@
       </c>
       <c r="I993" s="31"/>
     </row>
-    <row r="994" spans="1:9" ht="45">
+    <row r="994" spans="1:9">
       <c r="A994" s="29" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B994" s="30" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="C994" s="31" t="s">
-        <v>2091</v>
+        <v>2093</v>
       </c>
       <c r="D994" s="29"/>
       <c r="E994" s="29" t="s">
@@ -34010,13 +33626,13 @@
     </row>
     <row r="995" spans="1:9">
       <c r="A995" s="29" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B995" s="30" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="C995" s="31" t="s">
-        <v>2092</v>
+        <v>2094</v>
       </c>
       <c r="D995" s="29"/>
       <c r="E995" s="29" t="s">
@@ -34035,13 +33651,13 @@
     </row>
     <row r="996" spans="1:9">
       <c r="A996" s="29" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B996" s="30" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="C996" s="31" t="s">
-        <v>2093</v>
+        <v>2095</v>
       </c>
       <c r="D996" s="29"/>
       <c r="E996" s="29" t="s">
@@ -34060,13 +33676,13 @@
     </row>
     <row r="997" spans="1:9">
       <c r="A997" s="29" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B997" s="30" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="C997" s="31" t="s">
-        <v>2094</v>
+        <v>2096</v>
       </c>
       <c r="D997" s="29"/>
       <c r="E997" s="29" t="s">
@@ -34085,13 +33701,13 @@
     </row>
     <row r="998" spans="1:9">
       <c r="A998" s="29" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B998" s="30" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="C998" s="31" t="s">
-        <v>2095</v>
+        <v>2097</v>
       </c>
       <c r="D998" s="29"/>
       <c r="E998" s="29" t="s">
@@ -34110,13 +33726,13 @@
     </row>
     <row r="999" spans="1:9">
       <c r="A999" s="29" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B999" s="30" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="C999" s="31" t="s">
-        <v>2096</v>
+        <v>2098</v>
       </c>
       <c r="D999" s="29"/>
       <c r="E999" s="29" t="s">
@@ -34135,13 +33751,13 @@
     </row>
     <row r="1000" spans="1:9">
       <c r="A1000" s="29" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B1000" s="30" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="C1000" s="31" t="s">
-        <v>2097</v>
+        <v>2099</v>
       </c>
       <c r="D1000" s="29"/>
       <c r="E1000" s="29" t="s">
@@ -34160,13 +33776,13 @@
     </row>
     <row r="1001" spans="1:9">
       <c r="A1001" s="29" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="B1001" s="30" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="C1001" s="31" t="s">
-        <v>2098</v>
+        <v>2100</v>
       </c>
       <c r="D1001" s="29"/>
       <c r="E1001" s="29" t="s">
@@ -34185,13 +33801,13 @@
     </row>
     <row r="1002" spans="1:9">
       <c r="A1002" s="29" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B1002" s="30" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="C1002" s="31" t="s">
-        <v>2099</v>
+        <v>2101</v>
       </c>
       <c r="D1002" s="29"/>
       <c r="E1002" s="29" t="s">
@@ -34210,13 +33826,13 @@
     </row>
     <row r="1003" spans="1:9">
       <c r="A1003" s="29" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B1003" s="30" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="C1003" s="31" t="s">
-        <v>2100</v>
+        <v>2102</v>
       </c>
       <c r="D1003" s="29"/>
       <c r="E1003" s="29" t="s">
@@ -34235,13 +33851,13 @@
     </row>
     <row r="1004" spans="1:9">
       <c r="A1004" s="29" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B1004" s="30" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="C1004" s="31" t="s">
-        <v>2101</v>
+        <v>2103</v>
       </c>
       <c r="D1004" s="29"/>
       <c r="E1004" s="29" t="s">
@@ -34260,13 +33876,13 @@
     </row>
     <row r="1005" spans="1:9">
       <c r="A1005" s="29" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="B1005" s="30" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="C1005" s="31" t="s">
-        <v>2102</v>
+        <v>2104</v>
       </c>
       <c r="D1005" s="29"/>
       <c r="E1005" s="29" t="s">
@@ -34279,19 +33895,19 @@
         <v>15</v>
       </c>
       <c r="H1005" s="29" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I1005" s="31"/>
     </row>
     <row r="1006" spans="1:9">
       <c r="A1006" s="29" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B1006" s="30" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="C1006" s="31" t="s">
-        <v>2103</v>
+        <v>2105</v>
       </c>
       <c r="D1006" s="29"/>
       <c r="E1006" s="29" t="s">
@@ -34304,19 +33920,19 @@
         <v>15</v>
       </c>
       <c r="H1006" s="29" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I1006" s="31"/>
     </row>
     <row r="1007" spans="1:9">
       <c r="A1007" s="29" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="B1007" s="30" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="C1007" s="31" t="s">
-        <v>2104</v>
+        <v>2106</v>
       </c>
       <c r="D1007" s="29"/>
       <c r="E1007" s="29" t="s">
@@ -34335,13 +33951,13 @@
     </row>
     <row r="1008" spans="1:9">
       <c r="A1008" s="29" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="B1008" s="30" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="C1008" s="31" t="s">
-        <v>2105</v>
+        <v>2107</v>
       </c>
       <c r="D1008" s="29"/>
       <c r="E1008" s="29" t="s">
@@ -34360,13 +33976,13 @@
     </row>
     <row r="1009" spans="1:9">
       <c r="A1009" s="29" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="B1009" s="30" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C1009" s="31" t="s">
-        <v>2106</v>
+        <v>2108</v>
       </c>
       <c r="D1009" s="29"/>
       <c r="E1009" s="29" t="s">
@@ -34379,19 +33995,19 @@
         <v>15</v>
       </c>
       <c r="H1009" s="29" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I1009" s="31"/>
     </row>
     <row r="1010" spans="1:9">
       <c r="A1010" s="29" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B1010" s="30" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C1010" s="31" t="s">
-        <v>2107</v>
+        <v>2109</v>
       </c>
       <c r="D1010" s="29"/>
       <c r="E1010" s="29" t="s">
@@ -34404,70 +34020,25 @@
         <v>15</v>
       </c>
       <c r="H1010" s="29" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I1010" s="31"/>
     </row>
     <row r="1011" spans="1:9">
-      <c r="A1011" s="29" t="s">
-        <v>1030</v>
-      </c>
-      <c r="B1011" s="30" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C1011" s="31" t="s">
-        <v>2108</v>
-      </c>
-      <c r="D1011" s="29"/>
-      <c r="E1011" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1011" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1011" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1011" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1011" s="31"/>
+      <c r="A1011" s="3"/>
+      <c r="B1011" s="10"/>
     </row>
     <row r="1012" spans="1:9">
-      <c r="A1012" s="29" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B1012" s="30" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C1012" s="31" t="s">
-        <v>2109</v>
-      </c>
-      <c r="D1012" s="29"/>
-      <c r="E1012" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1012" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1012" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1012" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1012" s="31"/>
-    </row>
-    <row r="1013" spans="1:9">
-      <c r="A1013" s="3"/>
-      <c r="B1013" s="10"/>
-    </row>
-    <row r="1014" spans="1:9">
-      <c r="A1014" s="3"/>
-      <c r="B1014" s="10"/>
+      <c r="A1012" s="3"/>
+      <c r="B1012" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -34475,187 +34046,182 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E34:I397 E924:I924 A970:I1012 E399:I922 A20:H968 E926:I968">
-    <cfRule type="expression" dxfId="117" priority="81">
+  <conditionalFormatting sqref="E34:I397 E924:I924 A968:I1010 E399:I922 A20:H966 E926:I966">
+    <cfRule type="expression" dxfId="60" priority="81">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="82">
+    <cfRule type="expression" dxfId="59" priority="82">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="89">
+    <cfRule type="expression" dxfId="58" priority="89">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34:I397 E924:I924 A970:I1012 E399:I922 A20:H968 E926:I968">
-    <cfRule type="expression" dxfId="114" priority="35">
+  <conditionalFormatting sqref="E34:I397 E924:I924 A968:I1010 E399:I922 A20:H966 E926:I966">
+    <cfRule type="expression" dxfId="57" priority="35">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="36">
+    <cfRule type="expression" dxfId="56" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="37">
+    <cfRule type="expression" dxfId="55" priority="37">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F970:F1012 F20:F968">
-    <cfRule type="expression" dxfId="111" priority="41">
+  <conditionalFormatting sqref="F968:F1010 F20:F966">
+    <cfRule type="expression" dxfId="54" priority="41">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="42">
+    <cfRule type="expression" dxfId="53" priority="42">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I397 I924 I970:I1012 I926:I968">
-    <cfRule type="expression" dxfId="109" priority="32">
+  <conditionalFormatting sqref="I20:I397 I924 I968:I1010">
+    <cfRule type="expression" dxfId="52" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="33">
+    <cfRule type="expression" dxfId="51" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="34">
+    <cfRule type="expression" dxfId="50" priority="34">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I397 I924 I970:I1012 I926:I968">
-    <cfRule type="expression" dxfId="106" priority="29">
+  <conditionalFormatting sqref="I20:I397 I924 I968:I1010">
+    <cfRule type="expression" dxfId="49" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="30">
+    <cfRule type="expression" dxfId="48" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="31">
+    <cfRule type="expression" dxfId="47" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A969:D969 J969">
-    <cfRule type="expression" dxfId="103" priority="26">
+  <conditionalFormatting sqref="A967:D967 J967">
+    <cfRule type="expression" dxfId="46" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="27">
+    <cfRule type="expression" dxfId="45" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="28">
+    <cfRule type="expression" dxfId="44" priority="28">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A969:D969 J969">
-    <cfRule type="expression" dxfId="100" priority="23">
+  <conditionalFormatting sqref="A967:D967 J967">
+    <cfRule type="expression" dxfId="43" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="24">
+    <cfRule type="expression" dxfId="42" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="25">
+    <cfRule type="expression" dxfId="41" priority="25">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G969:I969 E969">
-    <cfRule type="expression" dxfId="97" priority="20">
+  <conditionalFormatting sqref="G967:I967 E967">
+    <cfRule type="expression" dxfId="40" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="21">
+    <cfRule type="expression" dxfId="39" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="22">
+    <cfRule type="expression" dxfId="38" priority="22">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G969:I969 E969">
-    <cfRule type="expression" dxfId="94" priority="17">
+  <conditionalFormatting sqref="G967:I967 E967">
+    <cfRule type="expression" dxfId="37" priority="17">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="18">
+    <cfRule type="expression" dxfId="36" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="19">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F969">
-    <cfRule type="expression" dxfId="91" priority="14">
+  <conditionalFormatting sqref="F967">
+    <cfRule type="expression" dxfId="34" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="15">
+    <cfRule type="expression" dxfId="33" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="16">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F969">
-    <cfRule type="expression" dxfId="88" priority="9">
+  <conditionalFormatting sqref="F967">
+    <cfRule type="expression" dxfId="31" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F969">
-    <cfRule type="expression" dxfId="85" priority="12">
-      <formula>NOT(VLOOKUP(F969,$A$12:$C$15,2,FALSE)="In")</formula>
+  <conditionalFormatting sqref="F967">
+    <cfRule type="expression" dxfId="28" priority="12">
+      <formula>NOT(VLOOKUP(F967,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="13">
-      <formula>(VLOOKUP(F969,$A$12:$C$15,2,FALSE)="In")</formula>
+    <cfRule type="expression" dxfId="27" priority="13">
+      <formula>(VLOOKUP(F967,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F969">
-    <cfRule type="expression" dxfId="83" priority="6">
+  <conditionalFormatting sqref="F967">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F969">
-    <cfRule type="expression" dxfId="80" priority="1">
+  <conditionalFormatting sqref="F967">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F969">
-    <cfRule type="expression" dxfId="77" priority="4">
-      <formula>NOT(VLOOKUP(F969,$A$12:$C$15,2,FALSE)="In")</formula>
+  <conditionalFormatting sqref="F967">
+    <cfRule type="expression" dxfId="20" priority="4">
+      <formula>NOT(VLOOKUP(F967,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="5">
-      <formula>(VLOOKUP(F969,$A$12:$C$15,2,FALSE)="In")</formula>
+    <cfRule type="expression" dxfId="19" priority="5">
+      <formula>(VLOOKUP(F967,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1012">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1010">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1012">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1010">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1012">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1010">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H970:H1012 H20:H968">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H968:H1010 H20:H966">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H969">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H967">
       <formula1>"Non-testable, Unverified, Adapter, Test Case, Deleted"</formula1>
     </dataValidation>
   </dataValidations>
@@ -34665,7 +34231,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B929:B1014 B19:B678 B681:B926" numberStoredAsText="1"/>
+    <ignoredError sqref="B927:B1012 B19:B680 B681:B926 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -34675,21 +34241,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -34738,16 +34289,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -34761,16 +34328,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix watchman error issues on MS-OXCNOTIF and MS-OXCPRPT
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
@@ -7423,6 +7423,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7446,21 +7461,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8527,7 +8527,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A400" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H405" sqref="H405"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -8580,127 +8582,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8713,12 +8715,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8731,12 +8733,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8749,12 +8751,12 @@
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8767,60 +8769,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -18580,7 +18582,7 @@
       <c r="B405" s="30" t="s">
         <v>1080</v>
       </c>
-      <c r="C405" s="31" t="s">
+      <c r="C405" s="20" t="s">
         <v>2257</v>
       </c>
       <c r="D405" s="29"/>
@@ -18594,7 +18596,7 @@
         <v>15</v>
       </c>
       <c r="H405" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I405" s="31"/>
     </row>
@@ -34034,11 +34036,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -34046,6 +34043,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E34:I397 E924:I924 A968:I1010 E399:I922 A20:H966 E926:I966">
@@ -34241,6 +34243,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -34289,15 +34300,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -34305,6 +34307,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34315,14 +34325,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
MS-OXCFXICS,MS-OXCROPS,MS-OXCRPC,MS-OXCPRPT: check up RS.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="180" windowWidth="15405" windowHeight="6780" tabRatio="570"/>
@@ -7258,7 +7258,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -8373,7 +8373,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8408,7 +8408,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8620,13 +8620,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C462" sqref="C462"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
@@ -34630,7 +34628,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B923:B1024 B19:B454 B601:B844" numberStoredAsText="1"/>
+    <ignoredError sqref="B922:B1024 B19:B921 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
[MS-OXCPRPT]/[MS-OXCRPC]/[MS-OXCROPS]: fix cases fail on E14
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="180" windowWidth="15405" windowHeight="6780" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7267" uniqueCount="2322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7268" uniqueCount="2322">
   <si>
     <t>Req ID</t>
   </si>
@@ -7556,21 +7556,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7588,6 +7573,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8406,6 +8406,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8441,6 +8458,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8673,127 +8707,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8806,12 +8840,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8824,12 +8858,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8842,12 +8876,12 @@
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8860,60 +8894,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="101.25" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="40" t="s">
         <v>2277</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -19924,7 +19958,7 @@
       </c>
       <c r="I454" s="31"/>
     </row>
-    <row r="455" spans="1:9" ht="30">
+    <row r="455" spans="1:9" ht="45">
       <c r="A455" s="22" t="s">
         <v>2286</v>
       </c>
@@ -19947,7 +19981,9 @@
       <c r="H455" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="I455" s="39"/>
+      <c r="I455" s="20" t="s">
+        <v>2231</v>
+      </c>
     </row>
     <row r="456" spans="1:9" ht="45">
       <c r="A456" s="22" t="s">
@@ -34431,6 +34467,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -34438,11 +34479,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E34:I397 E936:I936 A980:I1022 E938:I978 E399:I934 A20:H978">
@@ -34638,6 +34674,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -34686,12 +34728,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -34702,6 +34738,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34716,20 +34766,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
[MS-OXCPRPT] Task 1887644: Update RS according to latest version TD.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
@@ -7102,15 +7102,6 @@
     <t>[In Appendix A: Product Behavior] Implementation does implement the RopLockRegionStream ROP. (&lt;15&gt; Section 3.2.5.21: Exchange 2003 and Exchange 2007 implement the RopLockRegionStream ROP.)</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation does implement the RopUnlockRegionStream ROP. (&lt;16&gt; Section 3.2.5.22: Exchange 2003 and Exchange 2007 implement the RopUnlockRegionStream ROP ([MS-OXCROPS] section 2.2.9.10).)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does implement the RopWriteAndCommitStream ROP. (&lt;17&gt; Section 3.2.5.23: Exchange 2003 and Exchange 2007 implement the RopWriteAndCommitStream ROP ([MS-OXCROPS] section 2.2.9.11.))</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does implement the RopCloneStream ROP. (&lt;18&gt; Section 3.2.5.24: Exchange 2003 and Exchange 2007 implement the RopCloneStream ROP ([MS-OXCROPS] section 2.2.9.12).)</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation does return a NotSupported error (0x80040102) if the client attempts to open a stream on a public folder in any mode other than ReadOnly. (&lt;11&gt; Section 3.2.5.11: Exchange 2013 and above follow this behavior.)</t>
   </si>
   <si>
@@ -7253,6 +7244,15 @@
   </si>
   <si>
     <t>[In Processing RopCloneStream]When the server receives a RopCloneStream ROP request buffer ([MS-OXCROPS] section 2.2.9.13) from the client, the server parses the buffer.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does implement the RopUnlockRegionStream ROP. (&lt;16&gt; Section 3.2.5.22: Exchange 2003 and Exchange 2007 implement the RopUnlockRegionStream ROP ([MS-OXCROPS] section 2.2.9.11).)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does implement the RopWriteAndCommitStream ROP. (&lt;17&gt; Section 3.2.5.23: Exchange 2003 and Exchange 2007 implement the RopWriteAndCommitStream ROP ([MS-OXCROPS] section 2.2.9.12.))</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does implement the RopCloneStream ROP. (&lt;18&gt; Section 3.2.5.24: Exchange 2003 and Exchange 2007 implement the RopCloneStream ROP ([MS-OXCROPS] section 2.2.9.13).)</t>
   </si>
 </sst>
 </file>
@@ -7556,21 +7556,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7588,6 +7573,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8654,9 +8654,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -8698,7 +8696,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>2279</v>
+        <v>2276</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -8709,127 +8707,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8842,12 +8840,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8860,12 +8858,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8878,12 +8876,12 @@
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8896,60 +8894,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="101.25" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="40" t="s">
         <v>2236</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -19968,7 +19966,7 @@
         <v>1088</v>
       </c>
       <c r="C455" s="39" t="s">
-        <v>2276</v>
+        <v>2273</v>
       </c>
       <c r="D455" s="37"/>
       <c r="E455" s="29" t="s">
@@ -20199,7 +20197,7 @@
         <v>1090</v>
       </c>
       <c r="C464" s="39" t="s">
-        <v>2277</v>
+        <v>2274</v>
       </c>
       <c r="D464" s="37"/>
       <c r="E464" s="29" t="s">
@@ -20224,7 +20222,7 @@
         <v>1090</v>
       </c>
       <c r="C465" s="39" t="s">
-        <v>2278</v>
+        <v>2275</v>
       </c>
       <c r="D465" s="37"/>
       <c r="E465" s="29" t="s">
@@ -20249,7 +20247,7 @@
         <v>1091</v>
       </c>
       <c r="C466" s="20" t="s">
-        <v>2280</v>
+        <v>2277</v>
       </c>
       <c r="D466" s="29"/>
       <c r="E466" s="29" t="s">
@@ -20378,7 +20376,7 @@
         <v>1092</v>
       </c>
       <c r="C471" s="20" t="s">
-        <v>2281</v>
+        <v>2278</v>
       </c>
       <c r="D471" s="29"/>
       <c r="E471" s="29" t="s">
@@ -20403,7 +20401,7 @@
         <v>1093</v>
       </c>
       <c r="C472" s="20" t="s">
-        <v>2282</v>
+        <v>2279</v>
       </c>
       <c r="D472" s="29"/>
       <c r="E472" s="29" t="s">
@@ -20428,7 +20426,7 @@
         <v>1094</v>
       </c>
       <c r="C473" s="20" t="s">
-        <v>2283</v>
+        <v>2280</v>
       </c>
       <c r="D473" s="29"/>
       <c r="E473" s="29" t="s">
@@ -20557,7 +20555,7 @@
         <v>1095</v>
       </c>
       <c r="C478" s="20" t="s">
-        <v>2284</v>
+        <v>2281</v>
       </c>
       <c r="D478" s="29"/>
       <c r="E478" s="29" t="s">
@@ -20582,7 +20580,7 @@
         <v>1096</v>
       </c>
       <c r="C479" s="20" t="s">
-        <v>2285</v>
+        <v>2282</v>
       </c>
       <c r="D479" s="29"/>
       <c r="E479" s="29" t="s">
@@ -20682,7 +20680,7 @@
         <v>1097</v>
       </c>
       <c r="C483" s="20" t="s">
-        <v>2286</v>
+        <v>2283</v>
       </c>
       <c r="D483" s="29"/>
       <c r="E483" s="29" t="s">
@@ -20836,7 +20834,7 @@
         <v>1098</v>
       </c>
       <c r="C489" s="20" t="s">
-        <v>2287</v>
+        <v>2284</v>
       </c>
       <c r="D489" s="29"/>
       <c r="E489" s="29" t="s">
@@ -20936,7 +20934,7 @@
         <v>1099</v>
       </c>
       <c r="C493" s="20" t="s">
-        <v>2288</v>
+        <v>2285</v>
       </c>
       <c r="D493" s="29"/>
       <c r="E493" s="29" t="s">
@@ -21140,7 +21138,7 @@
         <v>1101</v>
       </c>
       <c r="C501" s="20" t="s">
-        <v>2289</v>
+        <v>2286</v>
       </c>
       <c r="D501" s="29"/>
       <c r="E501" s="29" t="s">
@@ -21415,7 +21413,7 @@
         <v>1102</v>
       </c>
       <c r="C512" s="20" t="s">
-        <v>2290</v>
+        <v>2287</v>
       </c>
       <c r="D512" s="29"/>
       <c r="E512" s="29" t="s">
@@ -21490,7 +21488,7 @@
         <v>1103</v>
       </c>
       <c r="C515" s="20" t="s">
-        <v>2291</v>
+        <v>2288</v>
       </c>
       <c r="D515" s="29"/>
       <c r="E515" s="29" t="s">
@@ -21619,7 +21617,7 @@
         <v>1104</v>
       </c>
       <c r="C520" s="20" t="s">
-        <v>2292</v>
+        <v>2289</v>
       </c>
       <c r="D520" s="29"/>
       <c r="E520" s="29" t="s">
@@ -21694,7 +21692,7 @@
         <v>1105</v>
       </c>
       <c r="C523" s="20" t="s">
-        <v>2293</v>
+        <v>2290</v>
       </c>
       <c r="D523" s="29"/>
       <c r="E523" s="29" t="s">
@@ -22344,7 +22342,7 @@
         <v>1109</v>
       </c>
       <c r="C549" s="20" t="s">
-        <v>2294</v>
+        <v>2291</v>
       </c>
       <c r="D549" s="29"/>
       <c r="E549" s="29" t="s">
@@ -22473,7 +22471,7 @@
         <v>1110</v>
       </c>
       <c r="C554" s="20" t="s">
-        <v>2295</v>
+        <v>2292</v>
       </c>
       <c r="D554" s="29"/>
       <c r="E554" s="29" t="s">
@@ -22723,7 +22721,7 @@
         <v>1111</v>
       </c>
       <c r="C564" s="20" t="s">
-        <v>2296</v>
+        <v>2293</v>
       </c>
       <c r="D564" s="29"/>
       <c r="E564" s="29" t="s">
@@ -22748,7 +22746,7 @@
         <v>1112</v>
       </c>
       <c r="C565" s="20" t="s">
-        <v>2297</v>
+        <v>2294</v>
       </c>
       <c r="D565" s="29"/>
       <c r="E565" s="29" t="s">
@@ -22877,7 +22875,7 @@
         <v>1113</v>
       </c>
       <c r="C570" s="20" t="s">
-        <v>2298</v>
+        <v>2295</v>
       </c>
       <c r="D570" s="29"/>
       <c r="E570" s="29" t="s">
@@ -23077,7 +23075,7 @@
         <v>1113</v>
       </c>
       <c r="C578" s="20" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="D578" s="29"/>
       <c r="E578" s="29" t="s">
@@ -23102,7 +23100,7 @@
         <v>1114</v>
       </c>
       <c r="C579" s="20" t="s">
-        <v>2299</v>
+        <v>2296</v>
       </c>
       <c r="D579" s="29"/>
       <c r="E579" s="29" t="s">
@@ -23127,7 +23125,7 @@
         <v>1115</v>
       </c>
       <c r="C580" s="20" t="s">
-        <v>2301</v>
+        <v>2298</v>
       </c>
       <c r="D580" s="29"/>
       <c r="E580" s="29" t="s">
@@ -23281,7 +23279,7 @@
         <v>1116</v>
       </c>
       <c r="C586" s="20" t="s">
-        <v>2302</v>
+        <v>2299</v>
       </c>
       <c r="D586" s="29"/>
       <c r="E586" s="29" t="s">
@@ -23381,7 +23379,7 @@
         <v>1117</v>
       </c>
       <c r="C590" s="20" t="s">
-        <v>2303</v>
+        <v>2300</v>
       </c>
       <c r="D590" s="29"/>
       <c r="E590" s="29" t="s">
@@ -23456,7 +23454,7 @@
         <v>2258</v>
       </c>
       <c r="C593" s="20" t="s">
-        <v>2304</v>
+        <v>2301</v>
       </c>
       <c r="D593" s="29"/>
       <c r="E593" s="29" t="s">
@@ -23610,7 +23608,7 @@
         <v>2259</v>
       </c>
       <c r="C599" s="20" t="s">
-        <v>2305</v>
+        <v>2302</v>
       </c>
       <c r="D599" s="29"/>
       <c r="E599" s="29" t="s">
@@ -23635,7 +23633,7 @@
         <v>2260</v>
       </c>
       <c r="C600" s="20" t="s">
-        <v>2306</v>
+        <v>2303</v>
       </c>
       <c r="D600" s="29"/>
       <c r="E600" s="29" t="s">
@@ -23835,7 +23833,7 @@
         <v>1118</v>
       </c>
       <c r="C608" s="20" t="s">
-        <v>2307</v>
+        <v>2304</v>
       </c>
       <c r="D608" s="29"/>
       <c r="E608" s="29" t="s">
@@ -24535,7 +24533,7 @@
         <v>1122</v>
       </c>
       <c r="C636" s="20" t="s">
-        <v>2308</v>
+        <v>2305</v>
       </c>
       <c r="D636" s="29"/>
       <c r="E636" s="29" t="s">
@@ -24760,7 +24758,7 @@
         <v>1123</v>
       </c>
       <c r="C645" s="20" t="s">
-        <v>2309</v>
+        <v>2306</v>
       </c>
       <c r="D645" s="29"/>
       <c r="E645" s="29" t="s">
@@ -24810,7 +24808,7 @@
         <v>1123</v>
       </c>
       <c r="C647" s="20" t="s">
-        <v>2310</v>
+        <v>2307</v>
       </c>
       <c r="D647" s="29"/>
       <c r="E647" s="29" t="s">
@@ -29735,7 +29733,7 @@
         <v>1138</v>
       </c>
       <c r="C842" s="20" t="s">
-        <v>2311</v>
+        <v>2308</v>
       </c>
       <c r="D842" s="29"/>
       <c r="E842" s="29" t="s">
@@ -29814,7 +29812,7 @@
         <v>1139</v>
       </c>
       <c r="C845" s="20" t="s">
-        <v>2312</v>
+        <v>2309</v>
       </c>
       <c r="D845" s="37"/>
       <c r="E845" s="37" t="s">
@@ -29839,7 +29837,7 @@
         <v>1140</v>
       </c>
       <c r="C846" s="20" t="s">
-        <v>2313</v>
+        <v>2310</v>
       </c>
       <c r="D846" s="29"/>
       <c r="E846" s="29" t="s">
@@ -29964,7 +29962,7 @@
         <v>1141</v>
       </c>
       <c r="C851" s="20" t="s">
-        <v>2314</v>
+        <v>2311</v>
       </c>
       <c r="D851" s="29"/>
       <c r="E851" s="29" t="s">
@@ -30089,7 +30087,7 @@
         <v>1142</v>
       </c>
       <c r="C856" s="20" t="s">
-        <v>2315</v>
+        <v>2312</v>
       </c>
       <c r="D856" s="29"/>
       <c r="E856" s="29" t="s">
@@ -30264,7 +30262,7 @@
         <v>1143</v>
       </c>
       <c r="C863" s="20" t="s">
-        <v>2316</v>
+        <v>2313</v>
       </c>
       <c r="D863" s="29"/>
       <c r="E863" s="29" t="s">
@@ -30493,7 +30491,7 @@
         <v>1144</v>
       </c>
       <c r="C872" s="20" t="s">
-        <v>2317</v>
+        <v>2314</v>
       </c>
       <c r="D872" s="29"/>
       <c r="E872" s="29" t="s">
@@ -30897,7 +30895,7 @@
         <v>1146</v>
       </c>
       <c r="C888" s="20" t="s">
-        <v>2318</v>
+        <v>2315</v>
       </c>
       <c r="D888" s="29"/>
       <c r="E888" s="29" t="s">
@@ -31199,7 +31197,7 @@
         <v>1147</v>
       </c>
       <c r="C900" s="20" t="s">
-        <v>2319</v>
+        <v>2316</v>
       </c>
       <c r="D900" s="29"/>
       <c r="E900" s="29" t="s">
@@ -31376,7 +31374,7 @@
         <v>1148</v>
       </c>
       <c r="C907" s="20" t="s">
-        <v>2320</v>
+        <v>2317</v>
       </c>
       <c r="D907" s="29"/>
       <c r="E907" s="29" t="s">
@@ -31553,7 +31551,7 @@
         <v>2265</v>
       </c>
       <c r="C914" s="20" t="s">
-        <v>2321</v>
+        <v>2318</v>
       </c>
       <c r="D914" s="29"/>
       <c r="E914" s="29" t="s">
@@ -32806,7 +32804,7 @@
         <v>1149</v>
       </c>
       <c r="C959" s="20" t="s">
-        <v>2275</v>
+        <v>2272</v>
       </c>
       <c r="D959" s="29" t="s">
         <v>2130</v>
@@ -32889,7 +32887,7 @@
         <v>1149</v>
       </c>
       <c r="C962" s="20" t="s">
-        <v>2274</v>
+        <v>2271</v>
       </c>
       <c r="D962" s="29" t="s">
         <v>2131</v>
@@ -33223,7 +33221,7 @@
         <v>1149</v>
       </c>
       <c r="C974" s="20" t="s">
-        <v>2271</v>
+        <v>2319</v>
       </c>
       <c r="D974" s="29" t="s">
         <v>2138</v>
@@ -33279,7 +33277,7 @@
         <v>1149</v>
       </c>
       <c r="C976" s="20" t="s">
-        <v>2272</v>
+        <v>2320</v>
       </c>
       <c r="D976" s="29" t="s">
         <v>2139</v>
@@ -33335,7 +33333,7 @@
         <v>1149</v>
       </c>
       <c r="C978" s="20" t="s">
-        <v>2273</v>
+        <v>2321</v>
       </c>
       <c r="D978" s="29" t="s">
         <v>2140</v>
@@ -34469,6 +34467,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -34476,11 +34479,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E34:I397 E936:I936 A980:I1022 E938:I978 E399:I934 A20:H978">
@@ -34676,6 +34674,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -34724,12 +34728,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -34740,6 +34738,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34754,20 +34766,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
MS-OXCPRPT: Update RS according to v20181001 document.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPRPT/MS-OXCPRPT_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75845891-9A43-4835-AD49-17671294A201}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2E1720-7C5C-4B65-93E9-2E29F62023DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="180" windowWidth="15405" windowHeight="6780" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -7253,7 +7253,8 @@
     <t>[In PidTagSearchKey Property] The PidTagSearchKey property ([MS-OXPROPS] section 2.991) contains a unique binary-comparable key that identifies an object for a search.</t>
   </si>
   <si>
-    <t>14.0</t>
+    <t>15.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -7261,14 +7262,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -7475,13 +7476,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -7514,7 +7515,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7557,21 +7558,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7590,9 +7576,24 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="61">
     <dxf>
@@ -8332,7 +8333,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -8659,15 +8660,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -8703,132 +8704,132 @@
         <v>26</v>
       </c>
       <c r="F3" s="12">
-        <v>43305</v>
+        <v>43374</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -8841,12 +8842,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -8859,12 +8860,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -8877,12 +8878,12 @@
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -8895,60 +8896,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="101.25" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="40" t="s">
         <v>2230</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -9107,7 +9108,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="25" spans="1:12" s="23" customFormat="1">
       <c r="A25" s="22" t="s">
         <v>48</v>
       </c>
@@ -9157,7 +9158,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="27" spans="1:12" s="23" customFormat="1">
       <c r="A27" s="22" t="s">
         <v>50</v>
       </c>
@@ -9182,7 +9183,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="28" spans="1:12" s="23" customFormat="1">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -9257,7 +9258,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="120">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="90">
       <c r="A31" s="22" t="s">
         <v>54</v>
       </c>
@@ -9334,7 +9335,7 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" ht="45">
+    <row r="34" spans="1:9" ht="30">
       <c r="A34" s="29" t="s">
         <v>57</v>
       </c>
@@ -9459,7 +9460,7 @@
       </c>
       <c r="I38" s="31"/>
     </row>
-    <row r="39" spans="1:9" ht="30">
+    <row r="39" spans="1:9">
       <c r="A39" s="29" t="s">
         <v>62</v>
       </c>
@@ -9484,7 +9485,7 @@
       </c>
       <c r="I39" s="31"/>
     </row>
-    <row r="40" spans="1:9" ht="30">
+    <row r="40" spans="1:9">
       <c r="A40" s="29" t="s">
         <v>63</v>
       </c>
@@ -9684,7 +9685,7 @@
       </c>
       <c r="I47" s="31"/>
     </row>
-    <row r="48" spans="1:9" ht="30">
+    <row r="48" spans="1:9">
       <c r="A48" s="29" t="s">
         <v>71</v>
       </c>
@@ -9709,7 +9710,7 @@
       </c>
       <c r="I48" s="31"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9">
       <c r="A49" s="29" t="s">
         <v>72</v>
       </c>
@@ -10184,7 +10185,7 @@
       </c>
       <c r="I67" s="31"/>
     </row>
-    <row r="68" spans="1:9" ht="45">
+    <row r="68" spans="1:9" ht="30">
       <c r="A68" s="29" t="s">
         <v>91</v>
       </c>
@@ -10234,7 +10235,7 @@
       </c>
       <c r="I69" s="31"/>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9">
       <c r="A70" s="29" t="s">
         <v>93</v>
       </c>
@@ -10259,7 +10260,7 @@
       </c>
       <c r="I70" s="31"/>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9">
       <c r="A71" s="29" t="s">
         <v>94</v>
       </c>
@@ -10284,7 +10285,7 @@
       </c>
       <c r="I71" s="31"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9">
       <c r="A72" s="29" t="s">
         <v>95</v>
       </c>
@@ -10309,7 +10310,7 @@
       </c>
       <c r="I72" s="31"/>
     </row>
-    <row r="73" spans="1:9" ht="30">
+    <row r="73" spans="1:9">
       <c r="A73" s="29" t="s">
         <v>96</v>
       </c>
@@ -10334,7 +10335,7 @@
       </c>
       <c r="I73" s="31"/>
     </row>
-    <row r="74" spans="1:9" ht="30">
+    <row r="74" spans="1:9">
       <c r="A74" s="29" t="s">
         <v>97</v>
       </c>
@@ -10359,7 +10360,7 @@
       </c>
       <c r="I74" s="31"/>
     </row>
-    <row r="75" spans="1:9" ht="30">
+    <row r="75" spans="1:9">
       <c r="A75" s="29" t="s">
         <v>98</v>
       </c>
@@ -10384,7 +10385,7 @@
       </c>
       <c r="I75" s="31"/>
     </row>
-    <row r="76" spans="1:9" ht="30">
+    <row r="76" spans="1:9">
       <c r="A76" s="29" t="s">
         <v>99</v>
       </c>
@@ -10709,7 +10710,7 @@
       </c>
       <c r="I88" s="31"/>
     </row>
-    <row r="89" spans="1:9" ht="45">
+    <row r="89" spans="1:9" ht="30">
       <c r="A89" s="29" t="s">
         <v>112</v>
       </c>
@@ -10934,7 +10935,7 @@
       </c>
       <c r="I97" s="31"/>
     </row>
-    <row r="98" spans="1:9" ht="45">
+    <row r="98" spans="1:9" ht="30">
       <c r="A98" s="29" t="s">
         <v>121</v>
       </c>
@@ -11036,7 +11037,7 @@
       </c>
       <c r="I101" s="31"/>
     </row>
-    <row r="102" spans="1:9" ht="60">
+    <row r="102" spans="1:9" ht="45">
       <c r="A102" s="29" t="s">
         <v>125</v>
       </c>
@@ -11186,7 +11187,7 @@
       </c>
       <c r="I107" s="31"/>
     </row>
-    <row r="108" spans="1:9" ht="45">
+    <row r="108" spans="1:9" ht="30">
       <c r="A108" s="29" t="s">
         <v>131</v>
       </c>
@@ -11211,7 +11212,7 @@
       </c>
       <c r="I108" s="31"/>
     </row>
-    <row r="109" spans="1:9" ht="45">
+    <row r="109" spans="1:9" ht="30">
       <c r="A109" s="29" t="s">
         <v>132</v>
       </c>
@@ -11286,7 +11287,7 @@
       </c>
       <c r="I111" s="31"/>
     </row>
-    <row r="112" spans="1:9" ht="30">
+    <row r="112" spans="1:9">
       <c r="A112" s="29" t="s">
         <v>135</v>
       </c>
@@ -11311,7 +11312,7 @@
       </c>
       <c r="I112" s="31"/>
     </row>
-    <row r="113" spans="1:9" ht="30">
+    <row r="113" spans="1:9">
       <c r="A113" s="29" t="s">
         <v>136</v>
       </c>
@@ -11336,7 +11337,7 @@
       </c>
       <c r="I113" s="31"/>
     </row>
-    <row r="114" spans="1:9" ht="30">
+    <row r="114" spans="1:9">
       <c r="A114" s="29" t="s">
         <v>137</v>
       </c>
@@ -11361,7 +11362,7 @@
       </c>
       <c r="I114" s="31"/>
     </row>
-    <row r="115" spans="1:9" ht="30">
+    <row r="115" spans="1:9">
       <c r="A115" s="29" t="s">
         <v>138</v>
       </c>
@@ -11486,7 +11487,7 @@
       </c>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="1:9" ht="45">
+    <row r="120" spans="1:9" ht="30">
       <c r="A120" s="29" t="s">
         <v>143</v>
       </c>
@@ -11513,7 +11514,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="45">
+    <row r="121" spans="1:9" ht="30">
       <c r="A121" s="29" t="s">
         <v>144</v>
       </c>
@@ -11538,7 +11539,7 @@
       </c>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="1:9" ht="45">
+    <row r="122" spans="1:9" ht="30">
       <c r="A122" s="29" t="s">
         <v>145</v>
       </c>
@@ -11613,7 +11614,7 @@
       </c>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="1:9" ht="45">
+    <row r="125" spans="1:9" ht="30">
       <c r="A125" s="29" t="s">
         <v>148</v>
       </c>
@@ -11763,7 +11764,7 @@
       </c>
       <c r="I130" s="31"/>
     </row>
-    <row r="131" spans="1:9" ht="60">
+    <row r="131" spans="1:9" ht="45">
       <c r="A131" s="29" t="s">
         <v>154</v>
       </c>
@@ -11788,7 +11789,7 @@
       </c>
       <c r="I131" s="31"/>
     </row>
-    <row r="132" spans="1:9" ht="45">
+    <row r="132" spans="1:9" ht="30">
       <c r="A132" s="29" t="s">
         <v>155</v>
       </c>
@@ -11813,7 +11814,7 @@
       </c>
       <c r="I132" s="31"/>
     </row>
-    <row r="133" spans="1:9" ht="30">
+    <row r="133" spans="1:9">
       <c r="A133" s="29" t="s">
         <v>156</v>
       </c>
@@ -11838,7 +11839,7 @@
       </c>
       <c r="I133" s="31"/>
     </row>
-    <row r="134" spans="1:9" ht="30">
+    <row r="134" spans="1:9">
       <c r="A134" s="29" t="s">
         <v>157</v>
       </c>
@@ -11863,7 +11864,7 @@
       </c>
       <c r="I134" s="31"/>
     </row>
-    <row r="135" spans="1:9" ht="30">
+    <row r="135" spans="1:9">
       <c r="A135" s="29" t="s">
         <v>158</v>
       </c>
@@ -11888,7 +11889,7 @@
       </c>
       <c r="I135" s="31"/>
     </row>
-    <row r="136" spans="1:9" ht="30">
+    <row r="136" spans="1:9">
       <c r="A136" s="29" t="s">
         <v>159</v>
       </c>
@@ -12138,7 +12139,7 @@
       </c>
       <c r="I145" s="31"/>
     </row>
-    <row r="146" spans="1:9" ht="30">
+    <row r="146" spans="1:9">
       <c r="A146" s="29" t="s">
         <v>169</v>
       </c>
@@ -12188,7 +12189,7 @@
       </c>
       <c r="I147" s="31"/>
     </row>
-    <row r="148" spans="1:9" ht="30">
+    <row r="148" spans="1:9">
       <c r="A148" s="29" t="s">
         <v>171</v>
       </c>
@@ -12338,7 +12339,7 @@
       </c>
       <c r="I153" s="31"/>
     </row>
-    <row r="154" spans="1:9" ht="45">
+    <row r="154" spans="1:9" ht="30">
       <c r="A154" s="29" t="s">
         <v>177</v>
       </c>
@@ -12613,7 +12614,7 @@
       </c>
       <c r="I164" s="31"/>
     </row>
-    <row r="165" spans="1:9" ht="75">
+    <row r="165" spans="1:9" ht="60">
       <c r="A165" s="29" t="s">
         <v>188</v>
       </c>
@@ -12663,7 +12664,7 @@
       </c>
       <c r="I166" s="31"/>
     </row>
-    <row r="167" spans="1:9" ht="45">
+    <row r="167" spans="1:9" ht="30">
       <c r="A167" s="29" t="s">
         <v>190</v>
       </c>
@@ -12688,7 +12689,7 @@
       </c>
       <c r="I167" s="31"/>
     </row>
-    <row r="168" spans="1:9" ht="30">
+    <row r="168" spans="1:9">
       <c r="A168" s="29" t="s">
         <v>191</v>
       </c>
@@ -12769,7 +12770,7 @@
       </c>
       <c r="I170" s="31"/>
     </row>
-    <row r="171" spans="1:9" ht="45">
+    <row r="171" spans="1:9" ht="30">
       <c r="A171" s="29" t="s">
         <v>194</v>
       </c>
@@ -12823,7 +12824,7 @@
       </c>
       <c r="I172" s="31"/>
     </row>
-    <row r="173" spans="1:9" ht="60">
+    <row r="173" spans="1:9" ht="45">
       <c r="A173" s="29" t="s">
         <v>196</v>
       </c>
@@ -13035,7 +13036,7 @@
       </c>
       <c r="I180" s="31"/>
     </row>
-    <row r="181" spans="1:9" ht="45">
+    <row r="181" spans="1:9" ht="30">
       <c r="A181" s="29" t="s">
         <v>204</v>
       </c>
@@ -13085,7 +13086,7 @@
       </c>
       <c r="I182" s="31"/>
     </row>
-    <row r="183" spans="1:9" ht="45">
+    <row r="183" spans="1:9" ht="30">
       <c r="A183" s="29" t="s">
         <v>206</v>
       </c>
@@ -13135,7 +13136,7 @@
       </c>
       <c r="I184" s="31"/>
     </row>
-    <row r="185" spans="1:9" ht="30">
+    <row r="185" spans="1:9">
       <c r="A185" s="29" t="s">
         <v>208</v>
       </c>
@@ -13214,7 +13215,7 @@
       </c>
       <c r="I187" s="31"/>
     </row>
-    <row r="188" spans="1:9" ht="30">
+    <row r="188" spans="1:9">
       <c r="A188" s="29" t="s">
         <v>211</v>
       </c>
@@ -13239,7 +13240,7 @@
       </c>
       <c r="I188" s="31"/>
     </row>
-    <row r="189" spans="1:9" ht="30">
+    <row r="189" spans="1:9">
       <c r="A189" s="29" t="s">
         <v>212</v>
       </c>
@@ -13264,7 +13265,7 @@
       </c>
       <c r="I189" s="31"/>
     </row>
-    <row r="190" spans="1:9" ht="30">
+    <row r="190" spans="1:9">
       <c r="A190" s="29" t="s">
         <v>213</v>
       </c>
@@ -13289,7 +13290,7 @@
       </c>
       <c r="I190" s="31"/>
     </row>
-    <row r="191" spans="1:9" ht="30">
+    <row r="191" spans="1:9">
       <c r="A191" s="29" t="s">
         <v>214</v>
       </c>
@@ -13639,7 +13640,7 @@
       </c>
       <c r="I204" s="31"/>
     </row>
-    <row r="205" spans="1:9" ht="75">
+    <row r="205" spans="1:9" ht="60">
       <c r="A205" s="29" t="s">
         <v>228</v>
       </c>
@@ -13689,7 +13690,7 @@
       </c>
       <c r="I206" s="31"/>
     </row>
-    <row r="207" spans="1:9" ht="45">
+    <row r="207" spans="1:9" ht="30">
       <c r="A207" s="29" t="s">
         <v>230</v>
       </c>
@@ -13741,7 +13742,7 @@
       </c>
       <c r="I208" s="31"/>
     </row>
-    <row r="209" spans="1:9" ht="30">
+    <row r="209" spans="1:9">
       <c r="A209" s="29" t="s">
         <v>232</v>
       </c>
@@ -13849,7 +13850,7 @@
       </c>
       <c r="I212" s="31"/>
     </row>
-    <row r="213" spans="1:9" ht="45">
+    <row r="213" spans="1:9" ht="30">
       <c r="A213" s="29" t="s">
         <v>236</v>
       </c>
@@ -13903,7 +13904,7 @@
       </c>
       <c r="I214" s="31"/>
     </row>
-    <row r="215" spans="1:9" ht="60">
+    <row r="215" spans="1:9" ht="45">
       <c r="A215" s="29" t="s">
         <v>238</v>
       </c>
@@ -14117,7 +14118,7 @@
       </c>
       <c r="I222" s="31"/>
     </row>
-    <row r="223" spans="1:9" ht="45">
+    <row r="223" spans="1:9" ht="30">
       <c r="A223" s="29" t="s">
         <v>246</v>
       </c>
@@ -14142,7 +14143,7 @@
       </c>
       <c r="I223" s="31"/>
     </row>
-    <row r="224" spans="1:9" ht="45">
+    <row r="224" spans="1:9" ht="30">
       <c r="A224" s="29" t="s">
         <v>247</v>
       </c>
@@ -14167,7 +14168,7 @@
       </c>
       <c r="I224" s="31"/>
     </row>
-    <row r="225" spans="1:9" ht="45">
+    <row r="225" spans="1:9" ht="30">
       <c r="A225" s="29" t="s">
         <v>248</v>
       </c>
@@ -14217,7 +14218,7 @@
       </c>
       <c r="I226" s="31"/>
     </row>
-    <row r="227" spans="1:9" ht="30">
+    <row r="227" spans="1:9">
       <c r="A227" s="29" t="s">
         <v>250</v>
       </c>
@@ -14323,7 +14324,7 @@
       </c>
       <c r="I230" s="31"/>
     </row>
-    <row r="231" spans="1:9" ht="45">
+    <row r="231" spans="1:9" ht="30">
       <c r="A231" s="29" t="s">
         <v>254</v>
       </c>
@@ -14475,7 +14476,7 @@
       </c>
       <c r="I236" s="31"/>
     </row>
-    <row r="237" spans="1:9" ht="45">
+    <row r="237" spans="1:9" ht="30">
       <c r="A237" s="29" t="s">
         <v>260</v>
       </c>
@@ -14550,7 +14551,7 @@
       </c>
       <c r="I239" s="31"/>
     </row>
-    <row r="240" spans="1:9" ht="30">
+    <row r="240" spans="1:9">
       <c r="A240" s="29" t="s">
         <v>263</v>
       </c>
@@ -14800,7 +14801,7 @@
       </c>
       <c r="I249" s="31"/>
     </row>
-    <row r="250" spans="1:9" ht="45">
+    <row r="250" spans="1:9" ht="30">
       <c r="A250" s="29" t="s">
         <v>273</v>
       </c>
@@ -15000,7 +15001,7 @@
       </c>
       <c r="I257" s="31"/>
     </row>
-    <row r="258" spans="1:9" ht="45">
+    <row r="258" spans="1:9" ht="30">
       <c r="A258" s="29" t="s">
         <v>281</v>
       </c>
@@ -15050,7 +15051,7 @@
       </c>
       <c r="I259" s="31"/>
     </row>
-    <row r="260" spans="1:9" ht="45">
+    <row r="260" spans="1:9" ht="30">
       <c r="A260" s="29" t="s">
         <v>283</v>
       </c>
@@ -15075,7 +15076,7 @@
       </c>
       <c r="I260" s="31"/>
     </row>
-    <row r="261" spans="1:9" ht="30">
+    <row r="261" spans="1:9">
       <c r="A261" s="29" t="s">
         <v>284</v>
       </c>
@@ -15100,7 +15101,7 @@
       </c>
       <c r="I261" s="31"/>
     </row>
-    <row r="262" spans="1:9" ht="30">
+    <row r="262" spans="1:9">
       <c r="A262" s="29" t="s">
         <v>285</v>
       </c>
@@ -15125,7 +15126,7 @@
       </c>
       <c r="I262" s="31"/>
     </row>
-    <row r="263" spans="1:9" ht="30">
+    <row r="263" spans="1:9">
       <c r="A263" s="29" t="s">
         <v>286</v>
       </c>
@@ -15150,7 +15151,7 @@
       </c>
       <c r="I263" s="31"/>
     </row>
-    <row r="264" spans="1:9" ht="30">
+    <row r="264" spans="1:9">
       <c r="A264" s="29" t="s">
         <v>287</v>
       </c>
@@ -15400,7 +15401,7 @@
       </c>
       <c r="I273" s="31"/>
     </row>
-    <row r="274" spans="1:9" ht="60">
+    <row r="274" spans="1:9" ht="45">
       <c r="A274" s="29" t="s">
         <v>297</v>
       </c>
@@ -15452,7 +15453,7 @@
       </c>
       <c r="I275" s="31"/>
     </row>
-    <row r="276" spans="1:9" ht="30">
+    <row r="276" spans="1:9">
       <c r="A276" s="29" t="s">
         <v>299</v>
       </c>
@@ -15552,7 +15553,7 @@
       </c>
       <c r="I279" s="31"/>
     </row>
-    <row r="280" spans="1:9" ht="45">
+    <row r="280" spans="1:9" ht="30">
       <c r="A280" s="29" t="s">
         <v>303</v>
       </c>
@@ -15802,7 +15803,7 @@
       </c>
       <c r="I289" s="31"/>
     </row>
-    <row r="290" spans="1:9" ht="45">
+    <row r="290" spans="1:9" ht="30">
       <c r="A290" s="29" t="s">
         <v>313</v>
       </c>
@@ -15877,7 +15878,7 @@
       </c>
       <c r="I292" s="31"/>
     </row>
-    <row r="293" spans="1:9" ht="45">
+    <row r="293" spans="1:9" ht="30">
       <c r="A293" s="29" t="s">
         <v>316</v>
       </c>
@@ -15927,7 +15928,7 @@
       </c>
       <c r="I294" s="31"/>
     </row>
-    <row r="295" spans="1:9" ht="45">
+    <row r="295" spans="1:9" ht="30">
       <c r="A295" s="29" t="s">
         <v>318</v>
       </c>
@@ -16227,7 +16228,7 @@
       </c>
       <c r="I306" s="31"/>
     </row>
-    <row r="307" spans="1:9" ht="30">
+    <row r="307" spans="1:9">
       <c r="A307" s="29" t="s">
         <v>330</v>
       </c>
@@ -16352,7 +16353,7 @@
       </c>
       <c r="I311" s="31"/>
     </row>
-    <row r="312" spans="1:9" ht="30">
+    <row r="312" spans="1:9">
       <c r="A312" s="29" t="s">
         <v>335</v>
       </c>
@@ -16377,7 +16378,7 @@
       </c>
       <c r="I312" s="31"/>
     </row>
-    <row r="313" spans="1:9" ht="60">
+    <row r="313" spans="1:9" ht="45">
       <c r="A313" s="29" t="s">
         <v>336</v>
       </c>
@@ -16856,7 +16857,7 @@
       </c>
       <c r="I331" s="31"/>
     </row>
-    <row r="332" spans="1:9" ht="45">
+    <row r="332" spans="1:9" ht="30">
       <c r="A332" s="29" t="s">
         <v>355</v>
       </c>
@@ -16906,7 +16907,7 @@
       </c>
       <c r="I333" s="31"/>
     </row>
-    <row r="334" spans="1:9" ht="45">
+    <row r="334" spans="1:9" ht="30">
       <c r="A334" s="29" t="s">
         <v>357</v>
       </c>
@@ -17131,7 +17132,7 @@
       </c>
       <c r="I342" s="31"/>
     </row>
-    <row r="343" spans="1:9" ht="45">
+    <row r="343" spans="1:9" ht="30">
       <c r="A343" s="29" t="s">
         <v>366</v>
       </c>
@@ -17208,7 +17209,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="346" spans="1:9" ht="45">
+    <row r="346" spans="1:9" ht="30">
       <c r="A346" s="29" t="s">
         <v>369</v>
       </c>
@@ -17233,7 +17234,7 @@
       </c>
       <c r="I346" s="31"/>
     </row>
-    <row r="347" spans="1:9" ht="45">
+    <row r="347" spans="1:9" ht="30">
       <c r="A347" s="29" t="s">
         <v>370</v>
       </c>
@@ -17258,7 +17259,7 @@
       </c>
       <c r="I347" s="31"/>
     </row>
-    <row r="348" spans="1:9" ht="30">
+    <row r="348" spans="1:9">
       <c r="A348" s="29" t="s">
         <v>371</v>
       </c>
@@ -17283,7 +17284,7 @@
       </c>
       <c r="I348" s="31"/>
     </row>
-    <row r="349" spans="1:9" ht="45">
+    <row r="349" spans="1:9" ht="30">
       <c r="A349" s="29" t="s">
         <v>372</v>
       </c>
@@ -17383,7 +17384,7 @@
       </c>
       <c r="I352" s="31"/>
     </row>
-    <row r="353" spans="1:9" ht="45">
+    <row r="353" spans="1:9" ht="30">
       <c r="A353" s="29" t="s">
         <v>376</v>
       </c>
@@ -17483,7 +17484,7 @@
       </c>
       <c r="I356" s="31"/>
     </row>
-    <row r="357" spans="1:9" ht="45">
+    <row r="357" spans="1:9" ht="30">
       <c r="A357" s="29" t="s">
         <v>380</v>
       </c>
@@ -17508,7 +17509,7 @@
       </c>
       <c r="I357" s="31"/>
     </row>
-    <row r="358" spans="1:9" ht="30">
+    <row r="358" spans="1:9">
       <c r="A358" s="29" t="s">
         <v>381</v>
       </c>
@@ -17533,7 +17534,7 @@
       </c>
       <c r="I358" s="31"/>
     </row>
-    <row r="359" spans="1:9" ht="45">
+    <row r="359" spans="1:9" ht="30">
       <c r="A359" s="29" t="s">
         <v>382</v>
       </c>
@@ -17658,7 +17659,7 @@
       </c>
       <c r="I363" s="31"/>
     </row>
-    <row r="364" spans="1:9" ht="45">
+    <row r="364" spans="1:9" ht="30">
       <c r="A364" s="29" t="s">
         <v>387</v>
       </c>
@@ -17683,7 +17684,7 @@
       </c>
       <c r="I364" s="31"/>
     </row>
-    <row r="365" spans="1:9" ht="45">
+    <row r="365" spans="1:9" ht="30">
       <c r="A365" s="29" t="s">
         <v>388</v>
       </c>
@@ -17708,7 +17709,7 @@
       </c>
       <c r="I365" s="31"/>
     </row>
-    <row r="366" spans="1:9" ht="45">
+    <row r="366" spans="1:9" ht="30">
       <c r="A366" s="29" t="s">
         <v>389</v>
       </c>
@@ -17733,7 +17734,7 @@
       </c>
       <c r="I366" s="31"/>
     </row>
-    <row r="367" spans="1:9" ht="45">
+    <row r="367" spans="1:9" ht="30">
       <c r="A367" s="29" t="s">
         <v>390</v>
       </c>
@@ -17983,7 +17984,7 @@
       </c>
       <c r="I376" s="31"/>
     </row>
-    <row r="377" spans="1:9" ht="45">
+    <row r="377" spans="1:9" ht="30">
       <c r="A377" s="29" t="s">
         <v>400</v>
       </c>
@@ -18058,7 +18059,7 @@
       </c>
       <c r="I379" s="31"/>
     </row>
-    <row r="380" spans="1:9" ht="30">
+    <row r="380" spans="1:9">
       <c r="A380" s="29" t="s">
         <v>403</v>
       </c>
@@ -18158,7 +18159,7 @@
       </c>
       <c r="I383" s="31"/>
     </row>
-    <row r="384" spans="1:9" ht="45">
+    <row r="384" spans="1:9" ht="30">
       <c r="A384" s="29" t="s">
         <v>407</v>
       </c>
@@ -18183,7 +18184,7 @@
       </c>
       <c r="I384" s="31"/>
     </row>
-    <row r="385" spans="1:9" ht="30">
+    <row r="385" spans="1:9">
       <c r="A385" s="29" t="s">
         <v>408</v>
       </c>
@@ -18408,7 +18409,7 @@
       </c>
       <c r="I393" s="31"/>
     </row>
-    <row r="394" spans="1:9" ht="30">
+    <row r="394" spans="1:9">
       <c r="A394" s="29" t="s">
         <v>417</v>
       </c>
@@ -18514,7 +18515,7 @@
       </c>
       <c r="I397" s="31"/>
     </row>
-    <row r="398" spans="1:9" ht="45">
+    <row r="398" spans="1:9" ht="42">
       <c r="A398" s="29" t="s">
         <v>421</v>
       </c>
@@ -18976,7 +18977,7 @@
       </c>
       <c r="I415" s="31"/>
     </row>
-    <row r="416" spans="1:9" ht="30">
+    <row r="416" spans="1:9">
       <c r="A416" s="29" t="s">
         <v>439</v>
       </c>
@@ -19226,7 +19227,7 @@
       </c>
       <c r="I425" s="31"/>
     </row>
-    <row r="426" spans="1:9" ht="45">
+    <row r="426" spans="1:9" ht="30">
       <c r="A426" s="29" t="s">
         <v>449</v>
       </c>
@@ -19405,7 +19406,7 @@
       </c>
       <c r="I432" s="31"/>
     </row>
-    <row r="433" spans="1:9" ht="45">
+    <row r="433" spans="1:9" ht="30">
       <c r="A433" s="29" t="s">
         <v>456</v>
       </c>
@@ -19680,7 +19681,7 @@
       </c>
       <c r="I443" s="31"/>
     </row>
-    <row r="444" spans="1:9" ht="45">
+    <row r="444" spans="1:9" ht="30">
       <c r="A444" s="29" t="s">
         <v>467</v>
       </c>
@@ -20013,7 +20014,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="457" spans="1:9" ht="30">
+    <row r="457" spans="1:9">
       <c r="A457" s="22" t="s">
         <v>2241</v>
       </c>
@@ -20090,7 +20091,7 @@
       </c>
       <c r="I459" s="39"/>
     </row>
-    <row r="460" spans="1:9" ht="45">
+    <row r="460" spans="1:9" ht="30">
       <c r="A460" s="22" t="s">
         <v>2244</v>
       </c>
@@ -20165,7 +20166,7 @@
       </c>
       <c r="I462" s="39"/>
     </row>
-    <row r="463" spans="1:9" ht="45">
+    <row r="463" spans="1:9" ht="30">
       <c r="A463" s="22" t="s">
         <v>2247</v>
       </c>
@@ -20265,7 +20266,7 @@
       </c>
       <c r="I466" s="31"/>
     </row>
-    <row r="467" spans="1:9" ht="45">
+    <row r="467" spans="1:9" ht="30">
       <c r="A467" s="29" t="s">
         <v>479</v>
       </c>
@@ -20444,7 +20445,7 @@
       </c>
       <c r="I473" s="31"/>
     </row>
-    <row r="474" spans="1:9" ht="45">
+    <row r="474" spans="1:9" ht="30">
       <c r="A474" s="29" t="s">
         <v>486</v>
       </c>
@@ -20648,7 +20649,7 @@
       </c>
       <c r="I481" s="31"/>
     </row>
-    <row r="482" spans="1:9" ht="30">
+    <row r="482" spans="1:9">
       <c r="A482" s="29" t="s">
         <v>494</v>
       </c>
@@ -20698,7 +20699,7 @@
       </c>
       <c r="I483" s="31"/>
     </row>
-    <row r="484" spans="1:9" ht="45">
+    <row r="484" spans="1:9" ht="30">
       <c r="A484" s="29" t="s">
         <v>496</v>
       </c>
@@ -20902,7 +20903,7 @@
       </c>
       <c r="I491" s="31"/>
     </row>
-    <row r="492" spans="1:9" ht="30">
+    <row r="492" spans="1:9">
       <c r="A492" s="29" t="s">
         <v>504</v>
       </c>
@@ -21027,7 +21028,7 @@
       </c>
       <c r="I496" s="31"/>
     </row>
-    <row r="497" spans="1:9" ht="45">
+    <row r="497" spans="1:9" ht="30">
       <c r="A497" s="29" t="s">
         <v>509</v>
       </c>
@@ -21506,7 +21507,7 @@
       </c>
       <c r="I515" s="31"/>
     </row>
-    <row r="516" spans="1:9" ht="45">
+    <row r="516" spans="1:9" ht="30">
       <c r="A516" s="29" t="s">
         <v>528</v>
       </c>
@@ -21735,7 +21736,7 @@
       </c>
       <c r="I524" s="31"/>
     </row>
-    <row r="525" spans="1:9" ht="45">
+    <row r="525" spans="1:9" ht="30">
       <c r="A525" s="29" t="s">
         <v>537</v>
       </c>
@@ -21785,7 +21786,7 @@
       </c>
       <c r="I526" s="31"/>
     </row>
-    <row r="527" spans="1:9" ht="45">
+    <row r="527" spans="1:9" ht="30">
       <c r="A527" s="29" t="s">
         <v>539</v>
       </c>
@@ -21935,7 +21936,7 @@
       </c>
       <c r="I532" s="31"/>
     </row>
-    <row r="533" spans="1:9" ht="45">
+    <row r="533" spans="1:9" ht="30">
       <c r="A533" s="29" t="s">
         <v>545</v>
       </c>
@@ -22010,7 +22011,7 @@
       </c>
       <c r="I535" s="31"/>
     </row>
-    <row r="536" spans="1:9" ht="30">
+    <row r="536" spans="1:9">
       <c r="A536" s="29" t="s">
         <v>548</v>
       </c>
@@ -22360,7 +22361,7 @@
       </c>
       <c r="I549" s="31"/>
     </row>
-    <row r="550" spans="1:9" ht="45">
+    <row r="550" spans="1:9" ht="30">
       <c r="A550" s="29" t="s">
         <v>562</v>
       </c>
@@ -22489,7 +22490,7 @@
       </c>
       <c r="I554" s="31"/>
     </row>
-    <row r="555" spans="1:9" ht="30">
+    <row r="555" spans="1:9">
       <c r="A555" s="29" t="s">
         <v>567</v>
       </c>
@@ -22514,7 +22515,7 @@
       </c>
       <c r="I555" s="31"/>
     </row>
-    <row r="556" spans="1:9" ht="45">
+    <row r="556" spans="1:9" ht="30">
       <c r="A556" s="29" t="s">
         <v>568</v>
       </c>
@@ -22539,7 +22540,7 @@
       </c>
       <c r="I556" s="31"/>
     </row>
-    <row r="557" spans="1:9" ht="30">
+    <row r="557" spans="1:9">
       <c r="A557" s="29" t="s">
         <v>569</v>
       </c>
@@ -22664,7 +22665,7 @@
       </c>
       <c r="I561" s="31"/>
     </row>
-    <row r="562" spans="1:9" ht="60">
+    <row r="562" spans="1:9" ht="45">
       <c r="A562" s="29" t="s">
         <v>574</v>
       </c>
@@ -22689,7 +22690,7 @@
       </c>
       <c r="I562" s="31"/>
     </row>
-    <row r="563" spans="1:9" ht="60">
+    <row r="563" spans="1:9" ht="45">
       <c r="A563" s="29" t="s">
         <v>575</v>
       </c>
@@ -22714,7 +22715,7 @@
       </c>
       <c r="I563" s="31"/>
     </row>
-    <row r="564" spans="1:9" ht="45">
+    <row r="564" spans="1:9" ht="30">
       <c r="A564" s="29" t="s">
         <v>576</v>
       </c>
@@ -22764,7 +22765,7 @@
       </c>
       <c r="I565" s="31"/>
     </row>
-    <row r="566" spans="1:9" ht="45">
+    <row r="566" spans="1:9" ht="30">
       <c r="A566" s="29" t="s">
         <v>578</v>
       </c>
@@ -22868,7 +22869,7 @@
       </c>
       <c r="I569" s="31"/>
     </row>
-    <row r="570" spans="1:9" ht="45">
+    <row r="570" spans="1:9" ht="30">
       <c r="A570" s="29" t="s">
         <v>582</v>
       </c>
@@ -22893,7 +22894,7 @@
       </c>
       <c r="I570" s="31"/>
     </row>
-    <row r="571" spans="1:9" ht="30">
+    <row r="571" spans="1:9">
       <c r="A571" s="29" t="s">
         <v>583</v>
       </c>
@@ -22943,7 +22944,7 @@
       </c>
       <c r="I572" s="31"/>
     </row>
-    <row r="573" spans="1:9" ht="30">
+    <row r="573" spans="1:9">
       <c r="A573" s="29" t="s">
         <v>585</v>
       </c>
@@ -23093,7 +23094,7 @@
       </c>
       <c r="I578" s="31"/>
     </row>
-    <row r="579" spans="1:9" ht="45">
+    <row r="579" spans="1:9" ht="30">
       <c r="A579" s="29" t="s">
         <v>591</v>
       </c>
@@ -23143,7 +23144,7 @@
       </c>
       <c r="I580" s="31"/>
     </row>
-    <row r="581" spans="1:9" ht="45">
+    <row r="581" spans="1:9" ht="30">
       <c r="A581" s="29" t="s">
         <v>593</v>
       </c>
@@ -23272,7 +23273,7 @@
       </c>
       <c r="I585" s="31"/>
     </row>
-    <row r="586" spans="1:9" ht="45">
+    <row r="586" spans="1:9" ht="30">
       <c r="A586" s="29" t="s">
         <v>598</v>
       </c>
@@ -23372,7 +23373,7 @@
       </c>
       <c r="I589" s="31"/>
     </row>
-    <row r="590" spans="1:9" ht="45">
+    <row r="590" spans="1:9" ht="30">
       <c r="A590" s="29" t="s">
         <v>602</v>
       </c>
@@ -23497,7 +23498,7 @@
       </c>
       <c r="I594" s="31"/>
     </row>
-    <row r="595" spans="1:9" ht="45">
+    <row r="595" spans="1:9" ht="30">
       <c r="A595" s="29" t="s">
         <v>607</v>
       </c>
@@ -23751,7 +23752,7 @@
       </c>
       <c r="I604" s="31"/>
     </row>
-    <row r="605" spans="1:9" ht="60">
+    <row r="605" spans="1:9" ht="45">
       <c r="A605" s="29" t="s">
         <v>617</v>
       </c>
@@ -23851,7 +23852,7 @@
       </c>
       <c r="I608" s="31"/>
     </row>
-    <row r="609" spans="1:9" ht="45">
+    <row r="609" spans="1:9" ht="30">
       <c r="A609" s="29" t="s">
         <v>621</v>
       </c>
@@ -23951,7 +23952,7 @@
       </c>
       <c r="I612" s="31"/>
     </row>
-    <row r="613" spans="1:9" ht="30">
+    <row r="613" spans="1:9">
       <c r="A613" s="29" t="s">
         <v>625</v>
       </c>
@@ -24001,7 +24002,7 @@
       </c>
       <c r="I614" s="31"/>
     </row>
-    <row r="615" spans="1:9" ht="45">
+    <row r="615" spans="1:9" ht="30">
       <c r="A615" s="29" t="s">
         <v>627</v>
       </c>
@@ -24176,7 +24177,7 @@
       </c>
       <c r="I621" s="31"/>
     </row>
-    <row r="622" spans="1:9" ht="45">
+    <row r="622" spans="1:9" ht="30">
       <c r="A622" s="29" t="s">
         <v>634</v>
       </c>
@@ -24376,7 +24377,7 @@
       </c>
       <c r="I629" s="31"/>
     </row>
-    <row r="630" spans="1:9" ht="60">
+    <row r="630" spans="1:9" ht="45">
       <c r="A630" s="29" t="s">
         <v>642</v>
       </c>
@@ -24401,7 +24402,7 @@
       </c>
       <c r="I630" s="31"/>
     </row>
-    <row r="631" spans="1:9" ht="75">
+    <row r="631" spans="1:9" ht="60">
       <c r="A631" s="29" t="s">
         <v>643</v>
       </c>
@@ -24526,7 +24527,7 @@
       </c>
       <c r="I635" s="31"/>
     </row>
-    <row r="636" spans="1:9" ht="45">
+    <row r="636" spans="1:9" ht="30">
       <c r="A636" s="29" t="s">
         <v>648</v>
       </c>
@@ -24751,7 +24752,7 @@
       </c>
       <c r="I644" s="31"/>
     </row>
-    <row r="645" spans="1:9" ht="45">
+    <row r="645" spans="1:9" ht="30">
       <c r="A645" s="29" t="s">
         <v>657</v>
       </c>
@@ -24951,7 +24952,7 @@
       </c>
       <c r="I652" s="31"/>
     </row>
-    <row r="653" spans="1:9" ht="60">
+    <row r="653" spans="1:9" ht="45">
       <c r="A653" s="29" t="s">
         <v>665</v>
       </c>
@@ -24976,7 +24977,7 @@
       </c>
       <c r="I653" s="31"/>
     </row>
-    <row r="654" spans="1:9" ht="60">
+    <row r="654" spans="1:9" ht="45">
       <c r="A654" s="29" t="s">
         <v>666</v>
       </c>
@@ -25001,7 +25002,7 @@
       </c>
       <c r="I654" s="31"/>
     </row>
-    <row r="655" spans="1:9" ht="60">
+    <row r="655" spans="1:9" ht="45">
       <c r="A655" s="29" t="s">
         <v>667</v>
       </c>
@@ -25026,7 +25027,7 @@
       </c>
       <c r="I655" s="31"/>
     </row>
-    <row r="656" spans="1:9" ht="60">
+    <row r="656" spans="1:9" ht="45">
       <c r="A656" s="29" t="s">
         <v>668</v>
       </c>
@@ -25051,7 +25052,7 @@
       </c>
       <c r="I656" s="31"/>
     </row>
-    <row r="657" spans="1:9" ht="60">
+    <row r="657" spans="1:9" ht="45">
       <c r="A657" s="29" t="s">
         <v>669</v>
       </c>
@@ -25076,7 +25077,7 @@
       </c>
       <c r="I657" s="31"/>
     </row>
-    <row r="658" spans="1:9" ht="60">
+    <row r="658" spans="1:9" ht="45">
       <c r="A658" s="29" t="s">
         <v>670</v>
       </c>
@@ -25101,7 +25102,7 @@
       </c>
       <c r="I658" s="31"/>
     </row>
-    <row r="659" spans="1:9" ht="60">
+    <row r="659" spans="1:9" ht="45">
       <c r="A659" s="29" t="s">
         <v>671</v>
       </c>
@@ -25126,7 +25127,7 @@
       </c>
       <c r="I659" s="31"/>
     </row>
-    <row r="660" spans="1:9" ht="60">
+    <row r="660" spans="1:9" ht="45">
       <c r="A660" s="29" t="s">
         <v>672</v>
       </c>
@@ -25151,7 +25152,7 @@
       </c>
       <c r="I660" s="31"/>
     </row>
-    <row r="661" spans="1:9" ht="60">
+    <row r="661" spans="1:9" ht="45">
       <c r="A661" s="29" t="s">
         <v>673</v>
       </c>
@@ -25176,7 +25177,7 @@
       </c>
       <c r="I661" s="31"/>
     </row>
-    <row r="662" spans="1:9" ht="60">
+    <row r="662" spans="1:9" ht="45">
       <c r="A662" s="29" t="s">
         <v>674</v>
       </c>
@@ -25276,7 +25277,7 @@
       </c>
       <c r="I665" s="31"/>
     </row>
-    <row r="666" spans="1:9" ht="45">
+    <row r="666" spans="1:9" ht="30">
       <c r="A666" s="29" t="s">
         <v>678</v>
       </c>
@@ -25351,7 +25352,7 @@
       </c>
       <c r="I668" s="31"/>
     </row>
-    <row r="669" spans="1:9" ht="45">
+    <row r="669" spans="1:9" ht="30">
       <c r="A669" s="29" t="s">
         <v>681</v>
       </c>
@@ -25451,7 +25452,7 @@
       </c>
       <c r="I672" s="31"/>
     </row>
-    <row r="673" spans="1:9" ht="45">
+    <row r="673" spans="1:9" ht="30">
       <c r="A673" s="29" t="s">
         <v>685</v>
       </c>
@@ -25584,7 +25585,7 @@
       </c>
       <c r="I677" s="31"/>
     </row>
-    <row r="678" spans="1:9" ht="45">
+    <row r="678" spans="1:9" ht="30">
       <c r="A678" s="29" t="s">
         <v>690</v>
       </c>
@@ -25609,7 +25610,7 @@
       </c>
       <c r="I678" s="31"/>
     </row>
-    <row r="679" spans="1:9" ht="45">
+    <row r="679" spans="1:9" ht="30">
       <c r="A679" s="29" t="s">
         <v>691</v>
       </c>
@@ -25634,7 +25635,7 @@
       </c>
       <c r="I679" s="31"/>
     </row>
-    <row r="680" spans="1:9" ht="45">
+    <row r="680" spans="1:9" ht="30">
       <c r="A680" s="29" t="s">
         <v>692</v>
       </c>
@@ -25684,7 +25685,7 @@
       </c>
       <c r="I681" s="31"/>
     </row>
-    <row r="682" spans="1:9" ht="45">
+    <row r="682" spans="1:9" ht="30">
       <c r="A682" s="29" t="s">
         <v>694</v>
       </c>
@@ -25809,7 +25810,7 @@
       </c>
       <c r="I686" s="31"/>
     </row>
-    <row r="687" spans="1:9" ht="45">
+    <row r="687" spans="1:9" ht="30">
       <c r="A687" s="29" t="s">
         <v>699</v>
       </c>
@@ -25861,7 +25862,7 @@
       </c>
       <c r="I688" s="31"/>
     </row>
-    <row r="689" spans="1:9" ht="30">
+    <row r="689" spans="1:9">
       <c r="A689" s="29" t="s">
         <v>701</v>
       </c>
@@ -25986,7 +25987,7 @@
       </c>
       <c r="I693" s="31"/>
     </row>
-    <row r="694" spans="1:9" ht="45">
+    <row r="694" spans="1:9" ht="30">
       <c r="A694" s="29" t="s">
         <v>704</v>
       </c>
@@ -26061,7 +26062,7 @@
       </c>
       <c r="I696" s="31"/>
     </row>
-    <row r="697" spans="1:9" ht="30">
+    <row r="697" spans="1:9">
       <c r="A697" s="29" t="s">
         <v>707</v>
       </c>
@@ -26186,7 +26187,7 @@
       </c>
       <c r="I701" s="31"/>
     </row>
-    <row r="702" spans="1:9" ht="30">
+    <row r="702" spans="1:9">
       <c r="A702" s="29" t="s">
         <v>712</v>
       </c>
@@ -26311,7 +26312,7 @@
       </c>
       <c r="I706" s="31"/>
     </row>
-    <row r="707" spans="1:9" ht="75">
+    <row r="707" spans="1:9" ht="60">
       <c r="A707" s="29" t="s">
         <v>717</v>
       </c>
@@ -26336,7 +26337,7 @@
       </c>
       <c r="I707" s="31"/>
     </row>
-    <row r="708" spans="1:9" ht="75">
+    <row r="708" spans="1:9" ht="60">
       <c r="A708" s="29" t="s">
         <v>718</v>
       </c>
@@ -26361,7 +26362,7 @@
       </c>
       <c r="I708" s="31"/>
     </row>
-    <row r="709" spans="1:9" ht="75">
+    <row r="709" spans="1:9" ht="60">
       <c r="A709" s="29" t="s">
         <v>719</v>
       </c>
@@ -26386,7 +26387,7 @@
       </c>
       <c r="I709" s="31"/>
     </row>
-    <row r="710" spans="1:9" ht="75">
+    <row r="710" spans="1:9" ht="60">
       <c r="A710" s="29" t="s">
         <v>720</v>
       </c>
@@ -26411,7 +26412,7 @@
       </c>
       <c r="I710" s="31"/>
     </row>
-    <row r="711" spans="1:9" ht="75">
+    <row r="711" spans="1:9" ht="60">
       <c r="A711" s="29" t="s">
         <v>721</v>
       </c>
@@ -26436,7 +26437,7 @@
       </c>
       <c r="I711" s="31"/>
     </row>
-    <row r="712" spans="1:9" ht="45">
+    <row r="712" spans="1:9" ht="30">
       <c r="A712" s="29" t="s">
         <v>722</v>
       </c>
@@ -26511,7 +26512,7 @@
       </c>
       <c r="I714" s="31"/>
     </row>
-    <row r="715" spans="1:9" ht="45">
+    <row r="715" spans="1:9" ht="30">
       <c r="A715" s="29" t="s">
         <v>725</v>
       </c>
@@ -26636,7 +26637,7 @@
       </c>
       <c r="I719" s="31"/>
     </row>
-    <row r="720" spans="1:9" ht="30">
+    <row r="720" spans="1:9">
       <c r="A720" s="29" t="s">
         <v>730</v>
       </c>
@@ -26786,7 +26787,7 @@
       </c>
       <c r="I725" s="31"/>
     </row>
-    <row r="726" spans="1:9" ht="45">
+    <row r="726" spans="1:9" ht="30">
       <c r="A726" s="29" t="s">
         <v>736</v>
       </c>
@@ -26838,7 +26839,7 @@
       </c>
       <c r="I727" s="31"/>
     </row>
-    <row r="728" spans="1:9" ht="60">
+    <row r="728" spans="1:9" ht="45">
       <c r="A728" s="29" t="s">
         <v>738</v>
       </c>
@@ -26913,7 +26914,7 @@
       </c>
       <c r="I730" s="31"/>
     </row>
-    <row r="731" spans="1:9" ht="60">
+    <row r="731" spans="1:9" ht="45">
       <c r="A731" s="29" t="s">
         <v>741</v>
       </c>
@@ -26990,7 +26991,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="734" spans="1:9" ht="45">
+    <row r="734" spans="1:9" ht="30">
       <c r="A734" s="29" t="s">
         <v>744</v>
       </c>
@@ -27115,7 +27116,7 @@
       </c>
       <c r="I738" s="31"/>
     </row>
-    <row r="739" spans="1:9" ht="60">
+    <row r="739" spans="1:9" ht="45">
       <c r="A739" s="29" t="s">
         <v>749</v>
       </c>
@@ -27140,7 +27141,7 @@
       </c>
       <c r="I739" s="31"/>
     </row>
-    <row r="740" spans="1:9" ht="45">
+    <row r="740" spans="1:9" ht="30">
       <c r="A740" s="29" t="s">
         <v>750</v>
       </c>
@@ -27165,7 +27166,7 @@
       </c>
       <c r="I740" s="31"/>
     </row>
-    <row r="741" spans="1:9" ht="60">
+    <row r="741" spans="1:9" ht="45">
       <c r="A741" s="29" t="s">
         <v>751</v>
       </c>
@@ -27190,7 +27191,7 @@
       </c>
       <c r="I741" s="31"/>
     </row>
-    <row r="742" spans="1:9" ht="45">
+    <row r="742" spans="1:9" ht="30">
       <c r="A742" s="29" t="s">
         <v>752</v>
       </c>
@@ -27269,7 +27270,7 @@
       </c>
       <c r="I744" s="31"/>
     </row>
-    <row r="745" spans="1:9" ht="30">
+    <row r="745" spans="1:9">
       <c r="A745" s="29" t="s">
         <v>755</v>
       </c>
@@ -27369,7 +27370,7 @@
       </c>
       <c r="I748" s="31"/>
     </row>
-    <row r="749" spans="1:9" ht="60">
+    <row r="749" spans="1:9" ht="45">
       <c r="A749" s="29" t="s">
         <v>759</v>
       </c>
@@ -27394,7 +27395,7 @@
       </c>
       <c r="I749" s="31"/>
     </row>
-    <row r="750" spans="1:9" ht="60">
+    <row r="750" spans="1:9" ht="45">
       <c r="A750" s="29" t="s">
         <v>760</v>
       </c>
@@ -27421,7 +27422,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="751" spans="1:9" ht="45">
+    <row r="751" spans="1:9" ht="30">
       <c r="A751" s="29" t="s">
         <v>761</v>
       </c>
@@ -27446,7 +27447,7 @@
       </c>
       <c r="I751" s="31"/>
     </row>
-    <row r="752" spans="1:9" ht="60">
+    <row r="752" spans="1:9" ht="45">
       <c r="A752" s="29" t="s">
         <v>762</v>
       </c>
@@ -27473,7 +27474,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="753" spans="1:9" ht="60">
+    <row r="753" spans="1:9" ht="45">
       <c r="A753" s="29" t="s">
         <v>763</v>
       </c>
@@ -27548,7 +27549,7 @@
       </c>
       <c r="I755" s="31"/>
     </row>
-    <row r="756" spans="1:9" ht="45">
+    <row r="756" spans="1:9" ht="30">
       <c r="A756" s="29" t="s">
         <v>766</v>
       </c>
@@ -27600,7 +27601,7 @@
       </c>
       <c r="I757" s="31"/>
     </row>
-    <row r="758" spans="1:9" ht="60">
+    <row r="758" spans="1:9" ht="45">
       <c r="A758" s="29" t="s">
         <v>768</v>
       </c>
@@ -27625,7 +27626,7 @@
       </c>
       <c r="I758" s="31"/>
     </row>
-    <row r="759" spans="1:9" ht="45">
+    <row r="759" spans="1:9" ht="30">
       <c r="A759" s="29" t="s">
         <v>769</v>
       </c>
@@ -27800,7 +27801,7 @@
       </c>
       <c r="I765" s="31"/>
     </row>
-    <row r="766" spans="1:9" ht="45">
+    <row r="766" spans="1:9" ht="30">
       <c r="A766" s="29" t="s">
         <v>776</v>
       </c>
@@ -27852,7 +27853,7 @@
       </c>
       <c r="I767" s="31"/>
     </row>
-    <row r="768" spans="1:9" ht="60">
+    <row r="768" spans="1:9" ht="45">
       <c r="A768" s="29" t="s">
         <v>778</v>
       </c>
@@ -27904,7 +27905,7 @@
       </c>
       <c r="I769" s="31"/>
     </row>
-    <row r="770" spans="1:9" ht="60">
+    <row r="770" spans="1:9" ht="45">
       <c r="A770" s="29" t="s">
         <v>780</v>
       </c>
@@ -27954,7 +27955,7 @@
       </c>
       <c r="I771" s="31"/>
     </row>
-    <row r="772" spans="1:9" ht="45">
+    <row r="772" spans="1:9" ht="30">
       <c r="A772" s="29" t="s">
         <v>782</v>
       </c>
@@ -27981,7 +27982,7 @@
         <v>2168</v>
       </c>
     </row>
-    <row r="773" spans="1:9" ht="60">
+    <row r="773" spans="1:9" ht="45">
       <c r="A773" s="29" t="s">
         <v>783</v>
       </c>
@@ -28033,7 +28034,7 @@
       </c>
       <c r="I774" s="31"/>
     </row>
-    <row r="775" spans="1:9" ht="60">
+    <row r="775" spans="1:9" ht="45">
       <c r="A775" s="29" t="s">
         <v>785</v>
       </c>
@@ -28058,7 +28059,7 @@
       </c>
       <c r="I775" s="31"/>
     </row>
-    <row r="776" spans="1:9" ht="45">
+    <row r="776" spans="1:9" ht="30">
       <c r="A776" s="29" t="s">
         <v>786</v>
       </c>
@@ -28108,7 +28109,7 @@
       </c>
       <c r="I777" s="31"/>
     </row>
-    <row r="778" spans="1:9" ht="45">
+    <row r="778" spans="1:9" ht="30">
       <c r="A778" s="29" t="s">
         <v>788</v>
       </c>
@@ -28160,7 +28161,7 @@
       </c>
       <c r="I779" s="31"/>
     </row>
-    <row r="780" spans="1:9" ht="60">
+    <row r="780" spans="1:9" ht="45">
       <c r="A780" s="29" t="s">
         <v>790</v>
       </c>
@@ -28187,7 +28188,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="781" spans="1:9" ht="45">
+    <row r="781" spans="1:9" ht="30">
       <c r="A781" s="29" t="s">
         <v>791</v>
       </c>
@@ -28241,7 +28242,7 @@
         <v>2173</v>
       </c>
     </row>
-    <row r="783" spans="1:9" ht="45">
+    <row r="783" spans="1:9" ht="30">
       <c r="A783" s="29" t="s">
         <v>793</v>
       </c>
@@ -28341,7 +28342,7 @@
       </c>
       <c r="I786" s="31"/>
     </row>
-    <row r="787" spans="1:9" ht="90">
+    <row r="787" spans="1:9" ht="75">
       <c r="A787" s="29" t="s">
         <v>797</v>
       </c>
@@ -28366,7 +28367,7 @@
       </c>
       <c r="I787" s="31"/>
     </row>
-    <row r="788" spans="1:9" ht="75">
+    <row r="788" spans="1:9" ht="60">
       <c r="A788" s="29" t="s">
         <v>798</v>
       </c>
@@ -28391,7 +28392,7 @@
       </c>
       <c r="I788" s="31"/>
     </row>
-    <row r="789" spans="1:9" ht="75">
+    <row r="789" spans="1:9" ht="60">
       <c r="A789" s="29" t="s">
         <v>799</v>
       </c>
@@ -28491,7 +28492,7 @@
       </c>
       <c r="I792" s="31"/>
     </row>
-    <row r="793" spans="1:9" ht="45">
+    <row r="793" spans="1:9" ht="30">
       <c r="A793" s="29" t="s">
         <v>803</v>
       </c>
@@ -28591,7 +28592,7 @@
       </c>
       <c r="I796" s="31"/>
     </row>
-    <row r="797" spans="1:9" ht="60">
+    <row r="797" spans="1:9" ht="45">
       <c r="A797" s="29" t="s">
         <v>807</v>
       </c>
@@ -28616,7 +28617,7 @@
       </c>
       <c r="I797" s="31"/>
     </row>
-    <row r="798" spans="1:9" ht="105">
+    <row r="798" spans="1:9" ht="90">
       <c r="A798" s="29" t="s">
         <v>808</v>
       </c>
@@ -28641,7 +28642,7 @@
       </c>
       <c r="I798" s="31"/>
     </row>
-    <row r="799" spans="1:9" ht="105">
+    <row r="799" spans="1:9" ht="90">
       <c r="A799" s="29" t="s">
         <v>809</v>
       </c>
@@ -28666,7 +28667,7 @@
       </c>
       <c r="I799" s="31"/>
     </row>
-    <row r="800" spans="1:9" ht="120">
+    <row r="800" spans="1:9" ht="105">
       <c r="A800" s="29" t="s">
         <v>810</v>
       </c>
@@ -28691,7 +28692,7 @@
       </c>
       <c r="I800" s="31"/>
     </row>
-    <row r="801" spans="1:9" ht="105">
+    <row r="801" spans="1:9" ht="90">
       <c r="A801" s="29" t="s">
         <v>811</v>
       </c>
@@ -28716,7 +28717,7 @@
       </c>
       <c r="I801" s="31"/>
     </row>
-    <row r="802" spans="1:9" ht="150">
+    <row r="802" spans="1:9" ht="120">
       <c r="A802" s="29" t="s">
         <v>812</v>
       </c>
@@ -28741,7 +28742,7 @@
       </c>
       <c r="I802" s="31"/>
     </row>
-    <row r="803" spans="1:9" ht="105">
+    <row r="803" spans="1:9" ht="90">
       <c r="A803" s="29" t="s">
         <v>813</v>
       </c>
@@ -28816,7 +28817,7 @@
       </c>
       <c r="I805" s="31"/>
     </row>
-    <row r="806" spans="1:9" ht="45">
+    <row r="806" spans="1:9" ht="30">
       <c r="A806" s="29" t="s">
         <v>816</v>
       </c>
@@ -28891,7 +28892,7 @@
       </c>
       <c r="I808" s="31"/>
     </row>
-    <row r="809" spans="1:9" ht="30">
+    <row r="809" spans="1:9">
       <c r="A809" s="29" t="s">
         <v>819</v>
       </c>
@@ -28991,7 +28992,7 @@
       </c>
       <c r="I812" s="31"/>
     </row>
-    <row r="813" spans="1:9" ht="60">
+    <row r="813" spans="1:9" ht="45">
       <c r="A813" s="29" t="s">
         <v>823</v>
       </c>
@@ -29093,7 +29094,7 @@
       </c>
       <c r="I816" s="31"/>
     </row>
-    <row r="817" spans="1:9" ht="30">
+    <row r="817" spans="1:9">
       <c r="A817" s="29" t="s">
         <v>827</v>
       </c>
@@ -29220,7 +29221,7 @@
       </c>
       <c r="I821" s="31"/>
     </row>
-    <row r="822" spans="1:9" ht="30">
+    <row r="822" spans="1:9">
       <c r="A822" s="29" t="s">
         <v>832</v>
       </c>
@@ -29295,7 +29296,7 @@
       </c>
       <c r="I824" s="31"/>
     </row>
-    <row r="825" spans="1:9" ht="30">
+    <row r="825" spans="1:9">
       <c r="A825" s="29" t="s">
         <v>835</v>
       </c>
@@ -29345,7 +29346,7 @@
       </c>
       <c r="I826" s="31"/>
     </row>
-    <row r="827" spans="1:9" ht="45">
+    <row r="827" spans="1:9" ht="30">
       <c r="A827" s="29" t="s">
         <v>837</v>
       </c>
@@ -29420,7 +29421,7 @@
       </c>
       <c r="I829" s="31"/>
     </row>
-    <row r="830" spans="1:9" ht="45">
+    <row r="830" spans="1:9" ht="30">
       <c r="A830" s="29" t="s">
         <v>840</v>
       </c>
@@ -29472,7 +29473,7 @@
       </c>
       <c r="I831" s="31"/>
     </row>
-    <row r="832" spans="1:9" ht="30">
+    <row r="832" spans="1:9">
       <c r="A832" s="29" t="s">
         <v>842</v>
       </c>
@@ -29547,7 +29548,7 @@
       </c>
       <c r="I834" s="31"/>
     </row>
-    <row r="835" spans="1:9" ht="60">
+    <row r="835" spans="1:9" ht="45">
       <c r="A835" s="29" t="s">
         <v>845</v>
       </c>
@@ -29624,7 +29625,7 @@
       </c>
       <c r="I837" s="31"/>
     </row>
-    <row r="838" spans="1:9" ht="45">
+    <row r="838" spans="1:9" ht="30">
       <c r="A838" s="29" t="s">
         <v>848</v>
       </c>
@@ -29676,7 +29677,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="840" spans="1:9" ht="45">
+    <row r="840" spans="1:9" ht="30">
       <c r="A840" s="29" t="s">
         <v>850</v>
       </c>
@@ -29751,7 +29752,7 @@
       </c>
       <c r="I842" s="31"/>
     </row>
-    <row r="843" spans="1:9" ht="45">
+    <row r="843" spans="1:9" ht="30">
       <c r="A843" s="29" t="s">
         <v>853</v>
       </c>
@@ -29778,7 +29779,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="844" spans="1:9" ht="45">
+    <row r="844" spans="1:9" ht="30">
       <c r="A844" s="29" t="s">
         <v>854</v>
       </c>
@@ -29805,7 +29806,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="845" spans="1:9" ht="60">
+    <row r="845" spans="1:9" ht="45">
       <c r="A845" s="22" t="s">
         <v>2258</v>
       </c>
@@ -29855,7 +29856,7 @@
       </c>
       <c r="I846" s="31"/>
     </row>
-    <row r="847" spans="1:9" ht="30">
+    <row r="847" spans="1:9">
       <c r="A847" s="29" t="s">
         <v>856</v>
       </c>
@@ -29930,7 +29931,7 @@
       </c>
       <c r="I849" s="31"/>
     </row>
-    <row r="850" spans="1:9" ht="45">
+    <row r="850" spans="1:9" ht="30">
       <c r="A850" s="29" t="s">
         <v>859</v>
       </c>
@@ -29980,7 +29981,7 @@
       </c>
       <c r="I851" s="31"/>
     </row>
-    <row r="852" spans="1:9" ht="30">
+    <row r="852" spans="1:9">
       <c r="A852" s="29" t="s">
         <v>861</v>
       </c>
@@ -30055,7 +30056,7 @@
       </c>
       <c r="I854" s="31"/>
     </row>
-    <row r="855" spans="1:9" ht="30">
+    <row r="855" spans="1:9">
       <c r="A855" s="29" t="s">
         <v>864</v>
       </c>
@@ -30105,7 +30106,7 @@
       </c>
       <c r="I856" s="31"/>
     </row>
-    <row r="857" spans="1:9" ht="30">
+    <row r="857" spans="1:9">
       <c r="A857" s="29" t="s">
         <v>866</v>
       </c>
@@ -30280,7 +30281,7 @@
       </c>
       <c r="I863" s="31"/>
     </row>
-    <row r="864" spans="1:9" ht="30">
+    <row r="864" spans="1:9">
       <c r="A864" s="29" t="s">
         <v>873</v>
       </c>
@@ -30380,7 +30381,7 @@
       </c>
       <c r="I867" s="31"/>
     </row>
-    <row r="868" spans="1:9" ht="45">
+    <row r="868" spans="1:9" ht="30">
       <c r="A868" s="29" t="s">
         <v>877</v>
       </c>
@@ -30430,7 +30431,7 @@
       </c>
       <c r="I869" s="31"/>
     </row>
-    <row r="870" spans="1:9" ht="45">
+    <row r="870" spans="1:9" ht="30">
       <c r="A870" s="29" t="s">
         <v>879</v>
       </c>
@@ -30457,7 +30458,7 @@
         <v>2180</v>
       </c>
     </row>
-    <row r="871" spans="1:9" ht="45">
+    <row r="871" spans="1:9" ht="30">
       <c r="A871" s="29" t="s">
         <v>880</v>
       </c>
@@ -30509,7 +30510,7 @@
       </c>
       <c r="I872" s="31"/>
     </row>
-    <row r="873" spans="1:9" ht="30">
+    <row r="873" spans="1:9">
       <c r="A873" s="29" t="s">
         <v>882</v>
       </c>
@@ -30584,7 +30585,7 @@
       </c>
       <c r="I875" s="31"/>
     </row>
-    <row r="876" spans="1:9" ht="45">
+    <row r="876" spans="1:9" ht="30">
       <c r="A876" s="29" t="s">
         <v>885</v>
       </c>
@@ -30661,7 +30662,7 @@
       </c>
       <c r="I878" s="31"/>
     </row>
-    <row r="879" spans="1:9" ht="45">
+    <row r="879" spans="1:9" ht="30">
       <c r="A879" s="29" t="s">
         <v>888</v>
       </c>
@@ -30888,7 +30889,7 @@
       </c>
       <c r="I887" s="31"/>
     </row>
-    <row r="888" spans="1:9" ht="45">
+    <row r="888" spans="1:9" ht="30">
       <c r="A888" s="29" t="s">
         <v>897</v>
       </c>
@@ -30988,7 +30989,7 @@
       </c>
       <c r="I891" s="31"/>
     </row>
-    <row r="892" spans="1:9" ht="45">
+    <row r="892" spans="1:9" ht="30">
       <c r="A892" s="29" t="s">
         <v>901</v>
       </c>
@@ -31040,7 +31041,7 @@
       </c>
       <c r="I893" s="31"/>
     </row>
-    <row r="894" spans="1:9" ht="45">
+    <row r="894" spans="1:9" ht="30">
       <c r="A894" s="29" t="s">
         <v>903</v>
       </c>
@@ -31065,7 +31066,7 @@
       </c>
       <c r="I894" s="31"/>
     </row>
-    <row r="895" spans="1:9" ht="60">
+    <row r="895" spans="1:9" ht="45">
       <c r="A895" s="29" t="s">
         <v>904</v>
       </c>
@@ -31090,7 +31091,7 @@
       </c>
       <c r="I895" s="31"/>
     </row>
-    <row r="896" spans="1:9" ht="45">
+    <row r="896" spans="1:9" ht="30">
       <c r="A896" s="29" t="s">
         <v>905</v>
       </c>
@@ -31140,7 +31141,7 @@
       </c>
       <c r="I897" s="31"/>
     </row>
-    <row r="898" spans="1:9" ht="60">
+    <row r="898" spans="1:9" ht="45">
       <c r="A898" s="29" t="s">
         <v>907</v>
       </c>
@@ -31165,7 +31166,7 @@
       </c>
       <c r="I898" s="31"/>
     </row>
-    <row r="899" spans="1:9" ht="45">
+    <row r="899" spans="1:9" ht="30">
       <c r="A899" s="29" t="s">
         <v>908</v>
       </c>
@@ -31190,7 +31191,7 @@
       </c>
       <c r="I899" s="31"/>
     </row>
-    <row r="900" spans="1:9" ht="45">
+    <row r="900" spans="1:9" ht="30">
       <c r="A900" s="29" t="s">
         <v>909</v>
       </c>
@@ -31290,7 +31291,7 @@
       </c>
       <c r="I903" s="31"/>
     </row>
-    <row r="904" spans="1:9" ht="45">
+    <row r="904" spans="1:9" ht="30">
       <c r="A904" s="29" t="s">
         <v>913</v>
       </c>
@@ -31342,7 +31343,7 @@
       </c>
       <c r="I905" s="31"/>
     </row>
-    <row r="906" spans="1:9" ht="45">
+    <row r="906" spans="1:9" ht="30">
       <c r="A906" s="29" t="s">
         <v>915</v>
       </c>
@@ -31367,7 +31368,7 @@
       </c>
       <c r="I906" s="31"/>
     </row>
-    <row r="907" spans="1:9" ht="45">
+    <row r="907" spans="1:9" ht="30">
       <c r="A907" s="29" t="s">
         <v>916</v>
       </c>
@@ -31467,7 +31468,7 @@
       </c>
       <c r="I910" s="31"/>
     </row>
-    <row r="911" spans="1:9" ht="45">
+    <row r="911" spans="1:9" ht="30">
       <c r="A911" s="29" t="s">
         <v>920</v>
       </c>
@@ -31569,7 +31570,7 @@
       </c>
       <c r="I914" s="31"/>
     </row>
-    <row r="915" spans="1:9" ht="30">
+    <row r="915" spans="1:9">
       <c r="A915" s="29" t="s">
         <v>924</v>
       </c>
@@ -31644,7 +31645,7 @@
       </c>
       <c r="I917" s="31"/>
     </row>
-    <row r="918" spans="1:9" ht="45">
+    <row r="918" spans="1:9" ht="30">
       <c r="A918" s="29" t="s">
         <v>927</v>
       </c>
@@ -31746,7 +31747,7 @@
       </c>
       <c r="I921" s="31"/>
     </row>
-    <row r="922" spans="1:9" ht="30">
+    <row r="922" spans="1:9">
       <c r="A922" s="29" t="s">
         <v>931</v>
       </c>
@@ -31821,7 +31822,7 @@
       </c>
       <c r="I924" s="31"/>
     </row>
-    <row r="925" spans="1:9" ht="45">
+    <row r="925" spans="1:9" ht="30">
       <c r="A925" s="29" t="s">
         <v>934</v>
       </c>
@@ -32076,7 +32077,7 @@
       </c>
       <c r="I933" s="31"/>
     </row>
-    <row r="934" spans="1:9" ht="45">
+    <row r="934" spans="1:9" ht="30">
       <c r="A934" s="29" t="s">
         <v>943</v>
       </c>
@@ -32161,7 +32162,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="937" spans="1:9" ht="60">
+    <row r="937" spans="1:9" ht="45">
       <c r="A937" s="29" t="s">
         <v>946</v>
       </c>
@@ -32393,7 +32394,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="945" spans="1:9" ht="60">
+    <row r="945" spans="1:9" ht="45">
       <c r="A945" s="29" t="s">
         <v>954</v>
       </c>
@@ -32596,7 +32597,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="952" spans="1:9" ht="60">
+    <row r="952" spans="1:9" ht="45">
       <c r="A952" s="29" t="s">
         <v>961</v>
       </c>
@@ -32768,7 +32769,7 @@
       </c>
       <c r="I957" s="31"/>
     </row>
-    <row r="958" spans="1:9" ht="60">
+    <row r="958" spans="1:9" ht="45">
       <c r="A958" s="29" t="s">
         <v>967</v>
       </c>
@@ -32797,7 +32798,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="959" spans="1:9" ht="60">
+    <row r="959" spans="1:9" ht="45">
       <c r="A959" s="29" t="s">
         <v>968</v>
       </c>
@@ -32853,7 +32854,7 @@
       </c>
       <c r="I960" s="31"/>
     </row>
-    <row r="961" spans="1:9" ht="60">
+    <row r="961" spans="1:9" ht="45">
       <c r="A961" s="29" t="s">
         <v>970</v>
       </c>
@@ -32992,7 +32993,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="966" spans="1:9" ht="45">
+    <row r="966" spans="1:9" ht="30">
       <c r="A966" s="29" t="s">
         <v>975</v>
       </c>
@@ -33383,7 +33384,7 @@
       </c>
       <c r="J979" s="31"/>
     </row>
-    <row r="980" spans="1:10" ht="30">
+    <row r="980" spans="1:10">
       <c r="A980" s="29" t="s">
         <v>988</v>
       </c>
@@ -33408,7 +33409,7 @@
       </c>
       <c r="I980" s="31"/>
     </row>
-    <row r="981" spans="1:10" ht="30">
+    <row r="981" spans="1:10">
       <c r="A981" s="29" t="s">
         <v>989</v>
       </c>
@@ -33433,7 +33434,7 @@
       </c>
       <c r="I981" s="31"/>
     </row>
-    <row r="982" spans="1:10" ht="30">
+    <row r="982" spans="1:10">
       <c r="A982" s="29" t="s">
         <v>990</v>
       </c>
@@ -33458,7 +33459,7 @@
       </c>
       <c r="I982" s="31"/>
     </row>
-    <row r="983" spans="1:10" ht="60">
+    <row r="983" spans="1:10" ht="45">
       <c r="A983" s="29" t="s">
         <v>991</v>
       </c>
@@ -33583,7 +33584,7 @@
       </c>
       <c r="I987" s="31"/>
     </row>
-    <row r="988" spans="1:10" ht="30">
+    <row r="988" spans="1:10">
       <c r="A988" s="29" t="s">
         <v>996</v>
       </c>
@@ -33608,7 +33609,7 @@
       </c>
       <c r="I988" s="31"/>
     </row>
-    <row r="989" spans="1:10" ht="45">
+    <row r="989" spans="1:10" ht="30">
       <c r="A989" s="29" t="s">
         <v>997</v>
       </c>
@@ -33658,7 +33659,7 @@
       </c>
       <c r="I990" s="31"/>
     </row>
-    <row r="991" spans="1:10" ht="30">
+    <row r="991" spans="1:10">
       <c r="A991" s="29" t="s">
         <v>999</v>
       </c>
@@ -33708,7 +33709,7 @@
       </c>
       <c r="I992" s="31"/>
     </row>
-    <row r="993" spans="1:9" ht="120">
+    <row r="993" spans="1:9" ht="105">
       <c r="A993" s="29" t="s">
         <v>1001</v>
       </c>
@@ -33783,7 +33784,7 @@
       </c>
       <c r="I995" s="31"/>
     </row>
-    <row r="996" spans="1:9" ht="30">
+    <row r="996" spans="1:9">
       <c r="A996" s="29" t="s">
         <v>1004</v>
       </c>
@@ -33883,7 +33884,7 @@
       </c>
       <c r="I999" s="31"/>
     </row>
-    <row r="1000" spans="1:9" ht="60">
+    <row r="1000" spans="1:9" ht="45">
       <c r="A1000" s="29" t="s">
         <v>1008</v>
       </c>
@@ -33983,7 +33984,7 @@
       </c>
       <c r="I1003" s="31"/>
     </row>
-    <row r="1004" spans="1:9" ht="45">
+    <row r="1004" spans="1:9" ht="30">
       <c r="A1004" s="29" t="s">
         <v>1012</v>
       </c>
@@ -34468,6 +34469,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -34475,11 +34481,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E34:I397 E936:I936 A980:I1022 E938:I978 E399:I934 A20:H978">
@@ -34665,7 +34666,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B922:B1024 B19:B921 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B922:B1024 B19:B921" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -34675,15 +34676,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -34732,6 +34724,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -34739,14 +34740,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34757,6 +34750,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>